<commit_message>
Update bond data with FRNK pricing source.
</commit_message>
<xml_diff>
--- a/CDNGovtBondPricesRaw.xlsx
+++ b/CDNGovtBondPricesRaw.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="-105" windowWidth="14850" windowHeight="12735" activeTab="1"/>
+    <workbookView xWindow="10395" yWindow="-105" windowWidth="3945" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="2" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t>Number of securities: 39</t>
   </si>
   <si>
-    <t>Currency: CAD</t>
-  </si>
-  <si>
-    <t>Created by  CALVIN MA ( GOVERNING COUNCIL OF UNIV OF TORONT )  on  01/25/2022 10:18:36 GMT-0500 (EST)</t>
+    <t>Currency: USD</t>
+  </si>
+  <si>
+    <t>Created by  CALVIN MA ( GOVERNING COUNCIL OF UNIV OF TORONT )  on  01/26/2022 09:37:17 GMT-0500 (EST)</t>
   </si>
   <si>
     <t>SRCH Criteria</t>
@@ -1076,10 +1076,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="33" borderId="0" xfId="26" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="26"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1201,12 +1200,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16404878468810349239</stp>
-        <tr r="H6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|16052265645252909906</stp>
         <tr r="G3" s="2"/>
       </tp>
@@ -1231,12 +1224,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10694321192837876646</stp>
-        <tr r="H36" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|11129068136639135333</stp>
         <tr r="D35" s="2"/>
       </tp>
@@ -1249,6 +1236,18 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|16890186005078062764</stp>
+        <tr r="H20" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11922935022805030777</stp>
+        <tr r="H16" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|13035054233781681889</stp>
         <tr r="B15" s="2"/>
       </tp>
@@ -1285,32 +1284,20 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12002977247352540421</stp>
-        <tr r="H28" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10115406292466731225</stp>
-        <tr r="H12" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|11571758974948591094</stp>
-        <tr r="H9" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12018287186819146855</stp>
-        <tr r="H22" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12225864559002291412</stp>
-        <tr r="H5" s="2"/>
+        <stp>BDH|17679879167287406702</stp>
+        <tr r="H25" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17606004267521143995</stp>
+        <tr r="H29" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13150668708589425531</stp>
+        <tr r="H21" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1351,12 +1338,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10739138010669673707</stp>
-        <tr r="H23" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|17838077417391039804</stp>
         <tr r="F19" s="2"/>
       </tp>
@@ -1411,6 +1392,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|16127898820244211720</stp>
+        <tr r="H36" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|10815916805127960241</stp>
         <tr r="C6" s="2"/>
       </tp>
@@ -1489,8 +1476,14 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12178049420985969887</stp>
-        <tr r="H27" s="2"/>
+        <stp>BDH|17832399536049622386</stp>
+        <tr r="H22" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13024152031044940835</stp>
+        <tr r="H35" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1531,6 +1524,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|14682171554996545473</stp>
+        <tr r="H26" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|13585203358514485344</stp>
         <tr r="B28" s="2"/>
       </tp>
@@ -1579,8 +1578,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15927443883299694317</stp>
-        <tr r="H17" s="2"/>
+        <stp>BDH|13539094309275733564</stp>
+        <tr r="H14" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1711,14 +1710,20 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14836360225475301177</stp>
-        <tr r="H29" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10890896599443354349</stp>
-        <tr r="H33" s="2"/>
+        <stp>BDH|17649906861688558196</stp>
+        <tr r="H5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|16278320559692497378</stp>
+        <tr r="H10" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11738731672091944137</stp>
+        <tr r="H11" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1753,12 +1758,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15880891466129108440</stp>
-        <tr r="H21" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|10972656469715486290</stp>
         <tr r="G31" s="2"/>
       </tp>
@@ -1813,14 +1812,14 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13363626822807539770</stp>
-        <tr r="H11" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|18006477137768253000</stp>
-        <tr r="H15" s="2"/>
+        <stp>BDH|10212163614740263737</stp>
+        <tr r="H1" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13099861902155819961</stp>
+        <tr r="H32" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1861,8 +1860,14 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12108811002557055921</stp>
-        <tr r="H26" s="2"/>
+        <stp>BDH|17347641231901491712</stp>
+        <tr r="H23" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11604076746307341675</stp>
+        <tr r="H4" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1906,18 +1911,6 @@
         <stp>BDP|15297699611431947658</stp>
         <tr r="B11" s="2"/>
       </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17007613656588991914</stp>
-        <tr r="H19" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|11786011945016526693</stp>
-        <tr r="H3" s="2"/>
-      </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
@@ -1941,6 +1934,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|1069490482816726712</stp>
+        <tr r="H30" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|3106376257488421167</stp>
         <tr r="B7" s="2"/>
       </tp>
@@ -1965,8 +1964,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8571808002734402874</stp>
-        <tr r="H7" s="2"/>
+        <stp>BDH|4616516580283106630</stp>
+        <tr r="H3" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -1983,6 +1982,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|6789811144651559655</stp>
+        <tr r="H7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|7209647007864461862</stp>
         <tr r="D30" s="2"/>
       </tp>
@@ -1995,18 +2000,18 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4960994127991583320</stp>
-        <tr r="H34" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|5311454641830122804</stp>
         <tr r="C29" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|9146272447805096773</stp>
+        <tr r="H31" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|9468085862295201789</stp>
         <tr r="D27" s="2"/>
       </tp>
@@ -2019,12 +2024,30 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|9365978902126804874</stp>
+        <tr r="H39" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2635387402036324917</stp>
+        <tr r="H6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|7063875043416053387</stp>
         <tr r="D21" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|8507288870017462494</stp>
+        <tr r="H27" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|7538727716178798714</stp>
         <tr r="F28" s="2"/>
       </tp>
@@ -2061,12 +2084,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5313841453256386199</stp>
-        <tr r="H8" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|7350028338768357352</stp>
         <tr r="E7" s="2"/>
       </tp>
@@ -2091,12 +2108,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|56561274212994247</stp>
-        <tr r="H1" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|3095783597242688724</stp>
         <tr r="F36" s="2"/>
       </tp>
@@ -2175,6 +2186,18 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|5513564619620262879</stp>
+        <tr r="H15" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|6812459685884090756</stp>
+        <tr r="H8" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|4992446779829882798</stp>
         <tr r="F7" s="2"/>
       </tp>
@@ -2211,12 +2234,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3610473609424649921</stp>
-        <tr r="H18" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|9446753131787784016</stp>
         <tr r="G6" s="2"/>
       </tp>
@@ -2229,6 +2246,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|1107073410519582342</stp>
+        <tr r="H9" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|6446297846253854892</stp>
         <tr r="C39" s="2"/>
       </tp>
@@ -2241,14 +2264,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2793236691833912146</stp>
-        <tr r="H4" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6108761739880975985</stp>
-        <tr r="H40" s="2"/>
+        <stp>BDH|9899632539275667277</stp>
+        <tr r="H38" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -2277,12 +2294,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4090392839561840161</stp>
-        <tr r="H37" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|2558648375610122781</stp>
         <tr r="B2" s="2"/>
       </tp>
@@ -2331,12 +2342,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9368860770910874366</stp>
-        <tr r="H10" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|2845229673120461257</stp>
         <tr r="D38" s="2"/>
       </tp>
@@ -2421,6 +2426,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|6093499115397617236</stp>
+        <tr r="H34" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|3326218959773044154</stp>
         <tr r="F33" s="2"/>
       </tp>
@@ -2439,8 +2450,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2102275041977462510</stp>
-        <tr r="H16" s="2"/>
+        <stp>BDH|3328349057647727442</stp>
+        <tr r="H24" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -2493,14 +2504,20 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|7557494997334697900</stp>
+        <tr r="H18" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|9094097717818512787</stp>
         <tr r="C23" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3917547236862092087</stp>
-        <tr r="H32" s="2"/>
+        <stp>BDH|6065857482376536731</stp>
+        <tr r="H40" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -2517,18 +2534,18 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7811461535722780584</stp>
-        <tr r="H14" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|5218502861087058664</stp>
         <tr r="E14" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|6239530491413954933</stp>
+        <tr r="H28" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|7356763479876534125</stp>
         <tr r="D8" s="2"/>
       </tp>
@@ -2547,6 +2564,18 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|2270691459428942930</stp>
+        <tr r="H17" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4475242769017948791</stp>
+        <tr r="H12" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|7327438979364183079</stp>
         <tr r="E17" s="2"/>
       </tp>
@@ -2565,13 +2594,7 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7370878945192129973</stp>
-        <tr r="H35" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|4380580636011148395</stp>
+        <stp>BDH|8917193872696394865</stp>
         <tr r="H13" s="2"/>
       </tp>
       <tp t="s">
@@ -2631,12 +2654,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3019304254142858554</stp>
-        <tr r="H38" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|1062056857624598282</stp>
         <tr r="B36" s="2"/>
       </tp>
@@ -2655,6 +2672,12 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|5865527624836030684</stp>
+        <tr r="H19" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|5252903323364311982</stp>
         <tr r="B19" s="2"/>
       </tp>
@@ -2673,12 +2696,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7988283078369014867</stp>
-        <tr r="H25" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|1801948255269465711</stp>
         <tr r="D33" s="2"/>
       </tp>
@@ -2691,24 +2708,30 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|1838293359394350182</stp>
+        <tr r="H33" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|6670675914241481319</stp>
         <tr r="D29" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
+        <stp>BDH|5891401194333931855</stp>
+        <tr r="H37" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
         <stp>BDP|3395477536512278579</stp>
         <tr r="G12" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7570297602743376588</stp>
-        <tr r="H30" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|17986130568836422</stp>
         <tr r="B34" s="2"/>
       </tp>
@@ -2721,12 +2744,6 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|536145580084452955</stp>
-        <tr r="H39" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|112862560859463301</stp>
         <tr r="G33" s="2"/>
       </tp>
@@ -2763,26 +2780,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|928461754300065143</stp>
-        <tr r="H20" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
         <stp>BDP|127877451523235257</stp>
         <tr r="D25" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|468301551128020274</stp>
-        <tr r="H24" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|511844764380400731</stp>
-        <tr r="H31" s="2"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
@@ -3090,46 +3089,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1">
-        <f>_xll.BDH($G$2&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "S", "Direction", "H", "Currency", "CAD","cols=11;rows=2")</f>
+        <f>_xll.BDH(G2&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "S", "Direction", "H", "Currency", "CAD", "PCS", "FRNK", "cols=11;rows=2")</f>
         <v>44571</v>
       </c>
       <c r="I1" s="1">
@@ -3192,37 +3192,37 @@
         <v>ZQ4084443</v>
       </c>
       <c r="H2">
-        <v>100.068</v>
+        <v>100.065</v>
       </c>
       <c r="I2">
-        <v>100.06399999999999</v>
+        <v>100.062</v>
       </c>
       <c r="J2">
-        <v>100.06</v>
+        <v>100.057</v>
       </c>
       <c r="K2">
-        <v>100.047</v>
+        <v>100.04600000000001</v>
       </c>
       <c r="L2">
-        <v>100.044</v>
+        <v>100.042</v>
       </c>
       <c r="M2">
-        <v>100.038</v>
+        <v>100.035</v>
       </c>
       <c r="N2">
-        <v>100.03400000000001</v>
+        <v>100.03</v>
       </c>
       <c r="O2">
-        <v>100.03</v>
+        <v>100.027</v>
       </c>
       <c r="P2">
-        <v>100.02200000000001</v>
+        <v>100.02</v>
       </c>
       <c r="Q2">
-        <v>100.01900000000001</v>
+        <v>100.032</v>
       </c>
       <c r="R2">
-        <v>100.01600000000001</v>
+        <v>100.014</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3254,38 +3254,38 @@
         <v>QZ8085933</v>
       </c>
       <c r="H3">
-        <f>_xll.BDH(G3&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.04300000000001</v>
+        <f>_xll.BDH(G3&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.038</v>
       </c>
       <c r="I3">
-        <v>100.042</v>
+        <v>100.036</v>
       </c>
       <c r="J3">
-        <v>100.035</v>
+        <v>100.032</v>
       </c>
       <c r="K3">
-        <v>100.03</v>
+        <v>100.02800000000001</v>
       </c>
       <c r="L3">
-        <v>100.027</v>
+        <v>100.02500000000001</v>
       </c>
       <c r="M3">
-        <v>100.01900000000001</v>
+        <v>100.015</v>
       </c>
       <c r="N3">
+        <v>100.01</v>
+      </c>
+      <c r="O3">
+        <v>100.011</v>
+      </c>
+      <c r="P3">
+        <v>100.011</v>
+      </c>
+      <c r="Q3">
         <v>100.014</v>
       </c>
-      <c r="O3">
-        <v>100.014</v>
-      </c>
-      <c r="P3">
+      <c r="R3">
         <v>100.01600000000001</v>
-      </c>
-      <c r="Q3">
-        <v>100.017</v>
-      </c>
-      <c r="R3">
-        <v>100.018</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -3317,38 +3317,38 @@
         <v>ZP6776824</v>
       </c>
       <c r="H4">
-        <f>_xll.BDH(G4&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.351</v>
+        <f>_xll.BDH(G4&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.349</v>
       </c>
       <c r="I4">
-        <v>100.346</v>
+        <v>100.34099999999999</v>
       </c>
       <c r="J4">
-        <v>100.33199999999999</v>
+        <v>100.333</v>
       </c>
       <c r="K4">
-        <v>100.322</v>
+        <v>100.32</v>
       </c>
       <c r="L4">
-        <v>100.306</v>
+        <v>100.309</v>
       </c>
       <c r="M4">
-        <v>100.288</v>
+        <v>100.28400000000001</v>
       </c>
       <c r="N4">
         <v>100.26900000000001</v>
       </c>
       <c r="O4">
-        <v>100.268</v>
+        <v>100.26600000000001</v>
       </c>
       <c r="P4">
+        <v>100.261</v>
+      </c>
+      <c r="Q4">
         <v>100.26900000000001</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>100.27</v>
-      </c>
-      <c r="R4">
-        <v>100.26900000000001</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -3380,38 +3380,38 @@
         <v>EI7672138</v>
       </c>
       <c r="H5">
-        <f>_xll.BDH(G5&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.90600000000001</v>
+        <f>_xll.BDH(G5&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.75700000000001</v>
       </c>
       <c r="I5">
-        <v>100.899</v>
+        <v>100.742</v>
       </c>
       <c r="J5">
-        <v>100.875</v>
+        <v>100.73399999999999</v>
       </c>
       <c r="K5">
-        <v>100.857</v>
+        <v>100.702</v>
       </c>
       <c r="L5">
-        <v>100.834</v>
+        <v>100.68899999999999</v>
       </c>
       <c r="M5">
-        <v>100.806</v>
+        <v>100.651</v>
       </c>
       <c r="N5">
-        <v>100.78</v>
+        <v>100.64</v>
       </c>
       <c r="O5">
-        <v>100.779</v>
+        <v>100.617</v>
       </c>
       <c r="P5">
-        <v>100.77200000000001</v>
+        <v>100.613</v>
       </c>
       <c r="Q5">
-        <v>100.77200000000001</v>
+        <v>100.627</v>
       </c>
       <c r="R5">
-        <v>100.767</v>
+        <v>100.621</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -3443,38 +3443,38 @@
         <v>135087UM4</v>
       </c>
       <c r="H6">
-        <f>_xll.BDH(G6&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>103.407</v>
+        <f>_xll.BDH(G6&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>103.395</v>
       </c>
       <c r="I6">
-        <v>103.38500000000001</v>
+        <v>103.36499999999999</v>
       </c>
       <c r="J6">
-        <v>103.333</v>
+        <v>103.334</v>
       </c>
       <c r="K6">
-        <v>103.27200000000001</v>
+        <v>103.256</v>
       </c>
       <c r="L6">
-        <v>103.22499999999999</v>
+        <v>103.221</v>
       </c>
       <c r="M6">
-        <v>103.18600000000001</v>
+        <v>103.16800000000001</v>
       </c>
       <c r="N6">
-        <v>103.13500000000001</v>
+        <v>103.13</v>
       </c>
       <c r="O6">
-        <v>103.117</v>
+        <v>103.105</v>
       </c>
       <c r="P6">
-        <v>103.053</v>
+        <v>103.038</v>
       </c>
       <c r="Q6">
-        <v>103.035</v>
+        <v>103.02800000000001</v>
       </c>
       <c r="R6">
-        <v>103.021</v>
+        <v>103.011</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -3506,38 +3506,38 @@
         <v>BJ2391222</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(G7&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.796999999999997</v>
+        <f>_xll.BDH(G7&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.793999999999997</v>
       </c>
       <c r="I7">
-        <v>99.8</v>
+        <v>99.786000000000001</v>
       </c>
       <c r="J7">
-        <v>99.772000000000006</v>
+        <v>99.775999999999996</v>
       </c>
       <c r="K7">
-        <v>99.774000000000001</v>
+        <v>99.77</v>
       </c>
       <c r="L7">
-        <v>99.754999999999995</v>
+        <v>99.759</v>
       </c>
       <c r="M7">
-        <v>99.724000000000004</v>
+        <v>99.718999999999994</v>
       </c>
       <c r="N7">
-        <v>99.694999999999993</v>
+        <v>99.697000000000003</v>
       </c>
       <c r="O7">
-        <v>99.703000000000003</v>
+        <v>99.700999999999993</v>
       </c>
       <c r="P7">
-        <v>99.724999999999994</v>
+        <v>99.713999999999999</v>
       </c>
       <c r="Q7">
-        <v>99.741</v>
+        <v>99.739000000000004</v>
       </c>
       <c r="R7">
-        <v>99.745999999999995</v>
+        <v>99.748000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3569,38 +3569,38 @@
         <v>AN1645463</v>
       </c>
       <c r="H8">
-        <f>_xll.BDH(G8&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.197</v>
+        <f>_xll.BDH(G8&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.19799999999999</v>
       </c>
       <c r="I8">
-        <v>100.196</v>
+        <v>100.187</v>
       </c>
       <c r="J8">
-        <v>100.16800000000001</v>
+        <v>100.17400000000001</v>
       </c>
       <c r="K8">
-        <v>100.166</v>
+        <v>100.16200000000001</v>
       </c>
       <c r="L8">
-        <v>100.134</v>
+        <v>100.145</v>
       </c>
       <c r="M8">
-        <v>100.1</v>
+        <v>100.09399999999999</v>
       </c>
       <c r="N8">
-        <v>100.066</v>
+        <v>100.069</v>
       </c>
       <c r="O8">
-        <v>100.074</v>
+        <v>100.071</v>
       </c>
       <c r="P8">
-        <v>100.09399999999999</v>
+        <v>100.081</v>
       </c>
       <c r="Q8">
-        <v>100.108</v>
+        <v>100.105</v>
       </c>
       <c r="R8">
-        <v>100.108</v>
+        <v>100.114</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3632,38 +3632,38 @@
         <v>BK9320544</v>
       </c>
       <c r="H9">
-        <f>_xll.BDH(G9&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.551000000000002</v>
+        <f>_xll.BDH(G9&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.552000000000007</v>
       </c>
       <c r="I9">
-        <v>99.554000000000002</v>
+        <v>99.540999999999997</v>
       </c>
       <c r="J9">
+        <v>99.527000000000001</v>
+      </c>
+      <c r="K9">
         <v>99.52</v>
       </c>
-      <c r="K9">
-        <v>99.525999999999996</v>
-      </c>
       <c r="L9">
-        <v>99.488</v>
+        <v>99.501000000000005</v>
       </c>
       <c r="M9">
-        <v>99.447999999999993</v>
+        <v>99.438999999999993</v>
       </c>
       <c r="N9">
-        <v>99.408000000000001</v>
+        <v>99.409000000000006</v>
       </c>
       <c r="O9">
         <v>99.415999999999997</v>
       </c>
       <c r="P9">
-        <v>99.448999999999998</v>
+        <v>99.432000000000002</v>
       </c>
       <c r="Q9">
-        <v>99.468000000000004</v>
+        <v>99.47</v>
       </c>
       <c r="R9">
-        <v>99.475999999999999</v>
+        <v>99.483999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3695,38 +3695,38 @@
         <v>BM0896381</v>
       </c>
       <c r="H10">
-        <f>_xll.BDH(G10&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.316000000000003</v>
+        <f>_xll.BDH(G10&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.307000000000002</v>
       </c>
       <c r="I10">
-        <v>99.320999999999998</v>
+        <v>99.301000000000002</v>
       </c>
       <c r="J10">
-        <v>99.278999999999996</v>
+        <v>99.281999999999996</v>
       </c>
       <c r="K10">
-        <v>99.284000000000006</v>
+        <v>99.274000000000001</v>
       </c>
       <c r="L10">
-        <v>99.233000000000004</v>
+        <v>99.251000000000005</v>
       </c>
       <c r="M10">
-        <v>99.179000000000002</v>
+        <v>99.17</v>
       </c>
       <c r="N10">
-        <v>99.125</v>
+        <v>99.132000000000005</v>
       </c>
       <c r="O10">
-        <v>99.132000000000005</v>
+        <v>99.14</v>
       </c>
       <c r="P10">
-        <v>99.168999999999997</v>
+        <v>99.156000000000006</v>
       </c>
       <c r="Q10">
-        <v>99.194999999999993</v>
+        <v>99.206000000000003</v>
       </c>
       <c r="R10">
-        <v>99.206000000000003</v>
+        <v>99.221999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -3758,38 +3758,38 @@
         <v>AP4340406</v>
       </c>
       <c r="H11">
-        <f>_xll.BDH(G11&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.944</v>
+        <f>_xll.BDH(G11&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.934</v>
       </c>
       <c r="I11">
-        <v>100.94199999999999</v>
+        <v>100.92100000000001</v>
       </c>
       <c r="J11">
-        <v>100.887</v>
+        <v>100.9</v>
       </c>
       <c r="K11">
-        <v>100.884</v>
+        <v>100.874</v>
       </c>
       <c r="L11">
-        <v>100.83199999999999</v>
+        <v>100.85299999999999</v>
       </c>
       <c r="M11">
-        <v>100.764</v>
+        <v>100.755</v>
       </c>
       <c r="N11">
-        <v>100.70699999999999</v>
+        <v>100.71</v>
       </c>
       <c r="O11">
-        <v>100.699</v>
+        <v>100.711</v>
       </c>
       <c r="P11">
-        <v>100.718</v>
+        <v>100.709</v>
       </c>
       <c r="Q11">
-        <v>100.739</v>
+        <v>100.748</v>
       </c>
       <c r="R11">
-        <v>100.746</v>
+        <v>100.76600000000001</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -3821,38 +3821,38 @@
         <v>BN9038405</v>
       </c>
       <c r="H12">
-        <f>_xll.BDH(G12&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.09</v>
+        <f>_xll.BDH(G12&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.081999999999994</v>
       </c>
       <c r="I12">
-        <v>99.094999999999999</v>
+        <v>99.073999999999998</v>
       </c>
       <c r="J12">
-        <v>99.043999999999997</v>
+        <v>99.055999999999997</v>
       </c>
       <c r="K12">
-        <v>99.054000000000002</v>
+        <v>99.042000000000002</v>
       </c>
       <c r="L12">
-        <v>98.991</v>
+        <v>99.018000000000001</v>
       </c>
       <c r="M12">
-        <v>98.923000000000002</v>
+        <v>98.912999999999997</v>
       </c>
       <c r="N12">
-        <v>98.855000000000004</v>
+        <v>98.864000000000004</v>
       </c>
       <c r="O12">
-        <v>98.858999999999995</v>
+        <v>98.873999999999995</v>
       </c>
       <c r="P12">
-        <v>98.888999999999996</v>
+        <v>98.882999999999996</v>
       </c>
       <c r="Q12">
-        <v>98.918000000000006</v>
+        <v>98.93</v>
       </c>
       <c r="R12">
-        <v>98.923000000000002</v>
+        <v>98.954999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -3884,38 +3884,38 @@
         <v>135087UT9</v>
       </c>
       <c r="H13">
-        <f>_xll.BDH(G13&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>109.66</v>
+        <f>_xll.BDH(G13&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>109.629</v>
       </c>
       <c r="I13">
-        <v>109.655</v>
+        <v>109.592</v>
       </c>
       <c r="J13">
-        <v>109.556</v>
+        <v>109.548</v>
       </c>
       <c r="K13">
-        <v>109.506</v>
+        <v>109.46899999999999</v>
       </c>
       <c r="L13">
-        <v>109.417</v>
+        <v>109.42100000000001</v>
       </c>
       <c r="M13">
-        <v>109.319</v>
+        <v>109.27800000000001</v>
       </c>
       <c r="N13">
-        <v>109.21899999999999</v>
+        <v>109.20099999999999</v>
       </c>
       <c r="O13">
-        <v>109.197</v>
+        <v>109.18899999999999</v>
       </c>
       <c r="P13">
-        <v>109.16200000000001</v>
+        <v>109.13200000000001</v>
       </c>
       <c r="Q13">
-        <v>109.17</v>
+        <v>109.161</v>
       </c>
       <c r="R13">
-        <v>109.173</v>
+        <v>109.169</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3947,38 +3947,38 @@
         <v>EJ2995995</v>
       </c>
       <c r="H14">
-        <f>_xll.BDH(G14&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.727</v>
+        <f>_xll.BDH(G14&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.70699999999999</v>
       </c>
       <c r="I14">
-        <v>100.723</v>
+        <v>100.687</v>
       </c>
       <c r="J14">
-        <v>100.663</v>
+        <v>100.678</v>
       </c>
       <c r="K14">
-        <v>100.66500000000001</v>
+        <v>100.637</v>
       </c>
       <c r="L14">
-        <v>100.593</v>
+        <v>100.6</v>
       </c>
       <c r="M14">
-        <v>100.514</v>
+        <v>100.485</v>
       </c>
       <c r="N14">
-        <v>100.437</v>
+        <v>100.432</v>
       </c>
       <c r="O14">
-        <v>100.437</v>
+        <v>100.43600000000001</v>
       </c>
       <c r="P14">
-        <v>100.45699999999999</v>
+        <v>100.443</v>
       </c>
       <c r="Q14">
-        <v>100.48099999999999</v>
+        <v>100.488</v>
       </c>
       <c r="R14">
-        <v>100.48699999999999</v>
+        <v>100.505</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -4010,38 +4010,38 @@
         <v>BP5161909</v>
       </c>
       <c r="H15">
-        <f>_xll.BDH(G15&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>98.820999999999998</v>
+        <f>_xll.BDH(G15&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>98.808000000000007</v>
       </c>
       <c r="I15">
-        <v>98.822000000000003</v>
+        <v>98.8</v>
       </c>
       <c r="J15">
-        <v>98.762</v>
+        <v>98.781000000000006</v>
       </c>
       <c r="K15">
-        <v>98.778000000000006</v>
+        <v>98.763000000000005</v>
       </c>
       <c r="L15">
-        <v>98.7</v>
+        <v>98.736000000000004</v>
       </c>
       <c r="M15">
-        <v>98.619</v>
+        <v>98.61</v>
       </c>
       <c r="N15">
-        <v>98.534999999999997</v>
+        <v>98.552999999999997</v>
       </c>
       <c r="O15">
-        <v>98.534000000000006</v>
+        <v>98.549000000000007</v>
       </c>
       <c r="P15">
-        <v>98.563999999999993</v>
+        <v>98.558000000000007</v>
       </c>
       <c r="Q15">
-        <v>98.6</v>
+        <v>98.611000000000004</v>
       </c>
       <c r="R15">
-        <v>98.605999999999995</v>
+        <v>98.635000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4073,38 +4073,38 @@
         <v>AS0892800</v>
       </c>
       <c r="H16">
-        <f>_xll.BDH(G16&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>101.574</v>
+        <f>_xll.BDH(G16&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>101.565</v>
       </c>
       <c r="I16">
-        <v>101.57299999999999</v>
+        <v>101.548</v>
       </c>
       <c r="J16">
-        <v>101.504</v>
+        <v>101.523</v>
       </c>
       <c r="K16">
-        <v>101.509</v>
+        <v>101.492</v>
       </c>
       <c r="L16">
-        <v>101.42100000000001</v>
+        <v>101.459</v>
       </c>
       <c r="M16">
-        <v>101.32599999999999</v>
+        <v>101.319</v>
       </c>
       <c r="N16">
-        <v>101.23</v>
+        <v>101.254</v>
       </c>
       <c r="O16">
-        <v>101.226</v>
+        <v>101.241</v>
       </c>
       <c r="P16">
-        <v>101.24299999999999</v>
+        <v>101.233</v>
       </c>
       <c r="Q16">
-        <v>101.268</v>
+        <v>101.286</v>
       </c>
       <c r="R16">
-        <v>101.271</v>
+        <v>101.30800000000001</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -4136,38 +4136,38 @@
         <v>BQ9098642</v>
       </c>
       <c r="H17">
-        <f>_xll.BDH(G17&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>98.978999999999999</v>
+        <f>_xll.BDH(G17&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>98.968000000000004</v>
       </c>
       <c r="I17">
-        <v>98.981999999999999</v>
+        <v>98.954999999999998</v>
       </c>
       <c r="J17">
+        <v>98.933999999999997</v>
+      </c>
+      <c r="K17">
         <v>98.911000000000001</v>
       </c>
-      <c r="K17">
-        <v>98.926000000000002</v>
-      </c>
       <c r="L17">
-        <v>98.835999999999999</v>
+        <v>98.878</v>
       </c>
       <c r="M17">
-        <v>98.742000000000004</v>
+        <v>98.731999999999999</v>
       </c>
       <c r="N17">
-        <v>98.64</v>
+        <v>98.665999999999997</v>
       </c>
       <c r="O17">
-        <v>98.638999999999996</v>
+        <v>98.653999999999996</v>
       </c>
       <c r="P17">
-        <v>98.668999999999997</v>
+        <v>98.661000000000001</v>
       </c>
       <c r="Q17">
-        <v>98.698999999999998</v>
+        <v>98.716999999999999</v>
       </c>
       <c r="R17">
-        <v>98.710999999999999</v>
+        <v>98.745999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -4199,38 +4199,38 @@
         <v>BS0586336</v>
       </c>
       <c r="H18">
-        <f>_xll.BDH(G18&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.224000000000004</v>
+        <f>_xll.BDH(G18&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.21</v>
       </c>
       <c r="I18">
-        <v>99.216999999999999</v>
+        <v>99.19</v>
       </c>
       <c r="J18">
-        <v>99.134</v>
+        <v>99.165000000000006</v>
       </c>
       <c r="K18">
-        <v>99.143000000000001</v>
+        <v>99.13</v>
       </c>
       <c r="L18">
-        <v>99.036000000000001</v>
+        <v>99.09</v>
       </c>
       <c r="M18">
-        <v>98.930999999999997</v>
+        <v>98.92</v>
       </c>
       <c r="N18">
-        <v>98.820999999999998</v>
+        <v>98.844999999999999</v>
       </c>
       <c r="O18">
-        <v>98.817999999999998</v>
+        <v>98.84</v>
       </c>
       <c r="P18">
-        <v>98.855000000000004</v>
+        <v>98.844999999999999</v>
       </c>
       <c r="Q18">
-        <v>98.903999999999996</v>
+        <v>98.92</v>
       </c>
       <c r="R18">
-        <v>98.915999999999997</v>
+        <v>98.954999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -4262,38 +4262,38 @@
         <v>AU8149901</v>
       </c>
       <c r="H19">
-        <f>_xll.BDH(G19&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>102.34</v>
+        <f>_xll.BDH(G19&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>102.32</v>
       </c>
       <c r="I19">
-        <v>102.331</v>
+        <v>102.29</v>
       </c>
       <c r="J19">
-        <v>102.238</v>
+        <v>102.28</v>
       </c>
       <c r="K19">
-        <v>102.242</v>
+        <v>102.23</v>
       </c>
       <c r="L19">
-        <v>102.126</v>
+        <v>102.18</v>
       </c>
       <c r="M19">
-        <v>102.008</v>
+        <v>102</v>
       </c>
       <c r="N19">
-        <v>101.883</v>
+        <v>101.91</v>
       </c>
       <c r="O19">
-        <v>101.877</v>
+        <v>101.89</v>
       </c>
       <c r="P19">
-        <v>101.901</v>
+        <v>101.89</v>
       </c>
       <c r="Q19">
-        <v>101.949</v>
+        <v>101.985</v>
       </c>
       <c r="R19">
-        <v>101.95099999999999</v>
+        <v>101.985</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -4325,38 +4325,38 @@
         <v>ZO9618760</v>
       </c>
       <c r="H20">
-        <f>_xll.BDH(G20&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>97.997</v>
+        <f>_xll.BDH(G20&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>97.974999999999994</v>
       </c>
       <c r="I20">
-        <v>97.992999999999995</v>
+        <v>97.96</v>
       </c>
       <c r="J20">
+        <v>97.93</v>
+      </c>
+      <c r="K20">
         <v>97.905000000000001</v>
       </c>
-      <c r="K20">
-        <v>97.927000000000007</v>
-      </c>
       <c r="L20">
-        <v>97.811000000000007</v>
+        <v>97.864999999999995</v>
       </c>
       <c r="M20">
-        <v>97.697999999999993</v>
+        <v>97.674999999999997</v>
       </c>
       <c r="N20">
-        <v>97.581000000000003</v>
+        <v>97.61</v>
       </c>
       <c r="O20">
-        <v>97.584000000000003</v>
+        <v>97.594999999999999</v>
       </c>
       <c r="P20">
-        <v>97.64</v>
+        <v>97.61</v>
       </c>
       <c r="Q20">
-        <v>97.695999999999998</v>
+        <v>97.715000000000003</v>
       </c>
       <c r="R20">
-        <v>97.712999999999994</v>
+        <v>97.754999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -4388,38 +4388,38 @@
         <v>EJ7362241</v>
       </c>
       <c r="H21">
-        <f>_xll.BDH(G21&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>103.048</v>
+        <f>_xll.BDH(G21&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>102.925</v>
       </c>
       <c r="I21">
-        <v>103.047</v>
+        <v>102.86</v>
       </c>
       <c r="J21">
-        <v>102.947</v>
+        <v>102.85</v>
       </c>
       <c r="K21">
-        <v>102.953</v>
+        <v>102.8</v>
       </c>
       <c r="L21">
-        <v>102.82</v>
+        <v>102.78</v>
       </c>
       <c r="M21">
-        <v>102.691</v>
+        <v>102.55500000000001</v>
       </c>
       <c r="N21">
-        <v>102.56399999999999</v>
+        <v>102.485</v>
       </c>
       <c r="O21">
-        <v>102.56399999999999</v>
+        <v>102.42</v>
       </c>
       <c r="P21">
-        <v>102.602</v>
+        <v>102.45</v>
       </c>
       <c r="Q21">
-        <v>102.65600000000001</v>
+        <v>102.53</v>
       </c>
       <c r="R21">
-        <v>102.666</v>
+        <v>102.61499999999999</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -4451,38 +4451,38 @@
         <v>ZS0489246</v>
       </c>
       <c r="H22">
-        <f>_xll.BDH(G22&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.69</v>
+        <f>_xll.BDH(G22&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.55</v>
       </c>
       <c r="I22">
-        <v>100.697</v>
+        <v>100.52</v>
       </c>
       <c r="J22">
-        <v>100.59399999999999</v>
+        <v>100.56</v>
       </c>
       <c r="K22">
-        <v>100.599</v>
+        <v>100.45</v>
       </c>
       <c r="L22">
-        <v>100.458</v>
+        <v>100.44</v>
       </c>
       <c r="M22">
-        <v>100.31399999999999</v>
+        <v>100.32</v>
       </c>
       <c r="N22">
-        <v>100.181</v>
+        <v>100.14</v>
       </c>
       <c r="O22">
-        <v>100.173</v>
+        <v>100.02</v>
       </c>
       <c r="P22">
-        <v>100.241</v>
+        <v>100.04</v>
       </c>
       <c r="Q22">
-        <v>100.313</v>
+        <v>100.11</v>
       </c>
       <c r="R22">
-        <v>100.334</v>
+        <v>100.18</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -4514,38 +4514,38 @@
         <v>BQ4678315</v>
       </c>
       <c r="H23">
-        <f>_xll.BDH(G23&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>98.59</v>
+        <f>_xll.BDH(G23&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>98.56</v>
       </c>
       <c r="I23">
-        <v>98.591999999999999</v>
+        <v>98.555000000000007</v>
       </c>
       <c r="J23">
-        <v>98.489000000000004</v>
+        <v>98.53</v>
       </c>
       <c r="K23">
-        <v>98.516000000000005</v>
+        <v>98.484999999999999</v>
       </c>
       <c r="L23">
-        <v>98.367999999999995</v>
+        <v>98.435000000000002</v>
       </c>
       <c r="M23">
-        <v>98.23</v>
+        <v>98.21</v>
       </c>
       <c r="N23">
-        <v>98.082999999999998</v>
+        <v>98.13</v>
       </c>
       <c r="O23">
-        <v>98.100999999999999</v>
+        <v>98.11</v>
       </c>
       <c r="P23">
-        <v>98.192999999999998</v>
+        <v>98.15</v>
       </c>
       <c r="Q23">
-        <v>98.289000000000001</v>
+        <v>98.29</v>
       </c>
       <c r="R23">
-        <v>98.302000000000007</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -4577,38 +4577,38 @@
         <v>ZQ0603485</v>
       </c>
       <c r="H24">
-        <f>_xll.BDH(G24&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>99.715999999999994</v>
+        <f>_xll.BDH(G24&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>99.65</v>
       </c>
       <c r="I24">
-        <v>99.716999999999999</v>
+        <v>99.655000000000001</v>
       </c>
       <c r="J24">
-        <v>99.602999999999994</v>
+        <v>99.614999999999995</v>
       </c>
       <c r="K24">
-        <v>99.646000000000001</v>
+        <v>99.584999999999994</v>
       </c>
       <c r="L24">
-        <v>99.456000000000003</v>
+        <v>99.5</v>
       </c>
       <c r="M24">
-        <v>99.302000000000007</v>
+        <v>99.254999999999995</v>
       </c>
       <c r="N24">
-        <v>99.113</v>
+        <v>99.125</v>
       </c>
       <c r="O24">
-        <v>99.108999999999995</v>
+        <v>99.105000000000004</v>
       </c>
       <c r="P24">
-        <v>99.192999999999998</v>
+        <v>99.12</v>
       </c>
       <c r="Q24">
-        <v>99.29</v>
+        <v>99.284999999999997</v>
       </c>
       <c r="R24">
-        <v>99.34</v>
+        <v>99.37</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -4640,38 +4640,38 @@
         <v>135087VH4</v>
       </c>
       <c r="H25">
-        <f>_xll.BDH(G25&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>125.22499999999999</v>
+        <f>_xll.BDH(G25&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>125.08</v>
       </c>
       <c r="I25">
-        <v>125.21899999999999</v>
+        <v>125.1</v>
       </c>
       <c r="J25">
-        <v>125.044</v>
+        <v>125.07</v>
       </c>
       <c r="K25">
-        <v>125.068</v>
+        <v>125.03</v>
       </c>
       <c r="L25">
-        <v>124.837</v>
+        <v>124.9</v>
       </c>
       <c r="M25">
-        <v>124.636</v>
+        <v>124.57</v>
       </c>
       <c r="N25">
-        <v>124.26600000000001</v>
+        <v>124.37</v>
       </c>
       <c r="O25">
-        <v>124.264</v>
+        <v>124.28</v>
       </c>
       <c r="P25">
-        <v>124.277</v>
+        <v>124.2</v>
       </c>
       <c r="Q25">
-        <v>124.393</v>
+        <v>124.39</v>
       </c>
       <c r="R25">
-        <v>124.376</v>
+        <v>124.51</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -4703,38 +4703,38 @@
         <v>EK3548485</v>
       </c>
       <c r="H26">
-        <f>_xll.BDH(G26&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>102.979</v>
+        <f>_xll.BDH(G26&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>102.92</v>
       </c>
       <c r="I26">
-        <v>102.99</v>
+        <v>102.95</v>
       </c>
       <c r="J26">
-        <v>102.866</v>
+        <v>102.905</v>
       </c>
       <c r="K26">
-        <v>102.93300000000001</v>
+        <v>102.905</v>
       </c>
       <c r="L26">
-        <v>102.741</v>
+        <v>102.81</v>
       </c>
       <c r="M26">
-        <v>102.557</v>
+        <v>102.535</v>
       </c>
       <c r="N26">
-        <v>102.268</v>
+        <v>102.355</v>
       </c>
       <c r="O26">
-        <v>102.252</v>
+        <v>102.30500000000001</v>
       </c>
       <c r="P26">
-        <v>102.33199999999999</v>
+        <v>102.295</v>
       </c>
       <c r="Q26">
-        <v>102.453</v>
+        <v>102.47</v>
       </c>
       <c r="R26">
-        <v>102.429</v>
+        <v>102.58</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -4766,38 +4766,38 @@
         <v>BH5185468</v>
       </c>
       <c r="H27">
-        <f>_xll.BDH(G27&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>96.826999999999998</v>
+        <f>_xll.BDH(G27&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>96.704999999999998</v>
       </c>
       <c r="I27">
-        <v>96.837999999999994</v>
+        <v>96.74</v>
       </c>
       <c r="J27">
-        <v>96.718000000000004</v>
+        <v>96.72</v>
       </c>
       <c r="K27">
-        <v>96.81</v>
+        <v>96.734999999999999</v>
       </c>
       <c r="L27">
-        <v>96.603999999999999</v>
+        <v>96.68</v>
       </c>
       <c r="M27">
-        <v>96.47</v>
+        <v>96.41</v>
       </c>
       <c r="N27">
-        <v>96.14</v>
+        <v>96.25</v>
       </c>
       <c r="O27">
-        <v>96.150999999999996</v>
+        <v>96.144999999999996</v>
       </c>
       <c r="P27">
-        <v>96.251000000000005</v>
+        <v>96.174999999999997</v>
       </c>
       <c r="Q27">
-        <v>96.369</v>
+        <v>96.334999999999994</v>
       </c>
       <c r="R27">
-        <v>96.346000000000004</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -4829,38 +4829,38 @@
         <v>ZO8493611</v>
       </c>
       <c r="H28">
-        <f>_xll.BDH(G28&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>95.188999999999993</v>
+        <f>_xll.BDH(G28&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>95.114999999999995</v>
       </c>
       <c r="I28">
-        <v>95.203999999999994</v>
+        <v>95.155000000000001</v>
       </c>
       <c r="J28">
-        <v>95.08</v>
+        <v>95.125</v>
       </c>
       <c r="K28">
-        <v>95.177999999999997</v>
+        <v>95.155000000000001</v>
       </c>
       <c r="L28">
-        <v>94.962000000000003</v>
+        <v>95.055000000000007</v>
       </c>
       <c r="M28">
-        <v>94.796999999999997</v>
+        <v>94.754999999999995</v>
       </c>
       <c r="N28">
-        <v>94.444999999999993</v>
+        <v>94.555000000000007</v>
       </c>
       <c r="O28">
-        <v>94.459000000000003</v>
+        <v>94.504999999999995</v>
       </c>
       <c r="P28">
-        <v>94.573999999999998</v>
+        <v>94.545000000000002</v>
       </c>
       <c r="Q28">
-        <v>94.712999999999994</v>
+        <v>94.73</v>
       </c>
       <c r="R28">
-        <v>94.691000000000003</v>
+        <v>94.875</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -4892,38 +4892,38 @@
         <v>UV3007514</v>
       </c>
       <c r="H29">
-        <f>_xll.BDH(G29&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>100.214</v>
+        <f>_xll.BDH(G29&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>100.13500000000001</v>
       </c>
       <c r="I29">
-        <v>100.221</v>
+        <v>100.175</v>
       </c>
       <c r="J29">
-        <v>100.089</v>
+        <v>100.14</v>
       </c>
       <c r="K29">
-        <v>100.19</v>
+        <v>100.155</v>
       </c>
       <c r="L29">
-        <v>99.947000000000003</v>
+        <v>100.04</v>
       </c>
       <c r="M29">
-        <v>99.763999999999996</v>
+        <v>99.71</v>
       </c>
       <c r="N29">
-        <v>99.375</v>
+        <v>99.545000000000002</v>
       </c>
       <c r="O29">
-        <v>99.387</v>
+        <v>99.435000000000002</v>
       </c>
       <c r="P29">
-        <v>99.503</v>
+        <v>99.44</v>
       </c>
       <c r="Q29">
-        <v>99.653000000000006</v>
+        <v>99.674999999999997</v>
       </c>
       <c r="R29">
-        <v>99.626999999999995</v>
+        <v>99.834999999999994</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -4955,38 +4955,38 @@
         <v>BP1003147</v>
       </c>
       <c r="H30">
-        <f>_xll.BDH(G30&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>97.75</v>
+        <f>_xll.BDH(G30&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>97.66</v>
       </c>
       <c r="I30">
-        <v>97.754000000000005</v>
+        <v>97.7</v>
       </c>
       <c r="J30">
-        <v>97.625</v>
+        <v>97.67</v>
       </c>
       <c r="K30">
-        <v>97.742999999999995</v>
+        <v>97.694999999999993</v>
       </c>
       <c r="L30">
-        <v>97.488</v>
+        <v>97.584999999999994</v>
       </c>
       <c r="M30">
-        <v>97.298000000000002</v>
+        <v>97.24</v>
       </c>
       <c r="N30">
-        <v>96.900999999999996</v>
+        <v>97.02</v>
       </c>
       <c r="O30">
-        <v>96.917000000000002</v>
+        <v>96.96</v>
       </c>
       <c r="P30">
-        <v>97.046000000000006</v>
+        <v>97</v>
       </c>
       <c r="Q30">
-        <v>97.212999999999994</v>
+        <v>97.224999999999994</v>
       </c>
       <c r="R30">
-        <v>97.192999999999998</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -5018,38 +5018,38 @@
         <v>BR9532150</v>
       </c>
       <c r="H31">
-        <f>_xll.BDH(G31&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>98.5</v>
+        <f>_xll.BDH(G31&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>98.41</v>
       </c>
       <c r="I31">
-        <v>98.5</v>
+        <v>98.45</v>
       </c>
       <c r="J31">
-        <v>98.394000000000005</v>
+        <v>98.41</v>
       </c>
       <c r="K31">
-        <v>98.504000000000005</v>
+        <v>98.454999999999998</v>
       </c>
       <c r="L31">
-        <v>98.22</v>
+        <v>98.33</v>
       </c>
       <c r="M31">
-        <v>98.019000000000005</v>
+        <v>97.954999999999998</v>
       </c>
       <c r="N31">
-        <v>97.591999999999999</v>
+        <v>97.715000000000003</v>
       </c>
       <c r="O31">
-        <v>97.628</v>
+        <v>97.665000000000006</v>
       </c>
       <c r="P31">
-        <v>97.760999999999996</v>
+        <v>97.71</v>
       </c>
       <c r="Q31">
-        <v>97.974000000000004</v>
+        <v>97.974999999999994</v>
       </c>
       <c r="R31">
-        <v>97.956999999999994</v>
+        <v>98.185000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -5081,38 +5081,38 @@
         <v>CC0002502</v>
       </c>
       <c r="H32">
-        <f>_xll.BDH(G32&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>133.434</v>
+        <f>_xll.BDH(G32&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>133.285</v>
       </c>
       <c r="I32">
-        <v>133.429</v>
+        <v>133.32</v>
       </c>
       <c r="J32">
-        <v>133.22800000000001</v>
+        <v>133.26</v>
       </c>
       <c r="K32">
-        <v>133.32499999999999</v>
+        <v>133.245</v>
       </c>
       <c r="L32">
-        <v>132.959</v>
+        <v>133.1</v>
       </c>
       <c r="M32">
-        <v>132.68700000000001</v>
+        <v>132.59</v>
       </c>
       <c r="N32">
-        <v>132.12</v>
+        <v>132.27000000000001</v>
       </c>
       <c r="O32">
-        <v>132.124</v>
+        <v>132.16</v>
       </c>
       <c r="P32">
-        <v>132.25399999999999</v>
+        <v>132.13999999999999</v>
       </c>
       <c r="Q32">
-        <v>132.471</v>
+        <v>132.47</v>
       </c>
       <c r="R32">
-        <v>132.41900000000001</v>
+        <v>132.69999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -5144,38 +5144,38 @@
         <v>QZ0744271</v>
       </c>
       <c r="H33">
-        <f>_xll.BDH(G33&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>97.391000000000005</v>
+        <f>_xll.BDH(G33&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>97.295000000000002</v>
       </c>
       <c r="I33">
-        <v>97.397000000000006</v>
+        <v>97.34</v>
       </c>
       <c r="J33">
-        <v>97.248999999999995</v>
+        <v>97.305000000000007</v>
       </c>
       <c r="K33">
-        <v>97.381</v>
+        <v>97.334999999999994</v>
       </c>
       <c r="L33">
-        <v>97.09</v>
+        <v>97.21</v>
       </c>
       <c r="M33">
-        <v>96.873000000000005</v>
+        <v>96.814999999999998</v>
       </c>
       <c r="N33">
-        <v>96.418000000000006</v>
+        <v>96.57</v>
       </c>
       <c r="O33">
-        <v>96.432000000000002</v>
+        <v>96.49</v>
       </c>
       <c r="P33">
-        <v>96.584000000000003</v>
+        <v>96.49</v>
       </c>
       <c r="Q33">
-        <v>96.781999999999996</v>
+        <v>96.795000000000002</v>
       </c>
       <c r="R33">
-        <v>96.754999999999995</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -5207,38 +5207,38 @@
         <v>AO5480923</v>
       </c>
       <c r="H34">
-        <f>_xll.BDH(G34&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>102.72499999999999</v>
+        <f>_xll.BDH(G34&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>102.545</v>
       </c>
       <c r="I34">
-        <v>102.699</v>
+        <v>102.595</v>
       </c>
       <c r="J34">
-        <v>102.527</v>
+        <v>102.535</v>
       </c>
       <c r="K34">
-        <v>102.691</v>
+        <v>102.565</v>
       </c>
       <c r="L34">
-        <v>102.321</v>
+        <v>102.42</v>
       </c>
       <c r="M34">
-        <v>102.07299999999999</v>
+        <v>101.94</v>
       </c>
       <c r="N34">
-        <v>101.521</v>
+        <v>101.63500000000001</v>
       </c>
       <c r="O34">
-        <v>101.55200000000001</v>
+        <v>101.55500000000001</v>
       </c>
       <c r="P34">
-        <v>101.756</v>
+        <v>101.63500000000001</v>
       </c>
       <c r="Q34">
-        <v>102.04600000000001</v>
+        <v>102.01</v>
       </c>
       <c r="R34">
-        <v>102.023</v>
+        <v>102.27</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -5270,38 +5270,38 @@
         <v>CC0020322</v>
       </c>
       <c r="H35">
-        <f>_xll.BDH(G35&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>128.98599999999999</v>
+        <f>_xll.BDH(G35&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>128.78</v>
       </c>
       <c r="I35">
-        <v>128.96899999999999</v>
+        <v>128.84</v>
       </c>
       <c r="J35">
-        <v>128.786</v>
+        <v>128.77000000000001</v>
       </c>
       <c r="K35">
-        <v>128.95099999999999</v>
+        <v>128.83000000000001</v>
       </c>
       <c r="L35">
-        <v>128.387</v>
+        <v>128.55000000000001</v>
       </c>
       <c r="M35">
-        <v>128.14400000000001</v>
+        <v>128.02000000000001</v>
       </c>
       <c r="N35">
-        <v>127.343</v>
+        <v>127.66</v>
       </c>
       <c r="O35">
-        <v>127.452</v>
+        <v>127.5</v>
       </c>
       <c r="P35">
-        <v>127.712</v>
+        <v>127.54</v>
       </c>
       <c r="Q35">
-        <v>128.06800000000001</v>
+        <v>128.04</v>
       </c>
       <c r="R35">
-        <v>127.95099999999999</v>
+        <v>128.41999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -5333,38 +5333,38 @@
         <v>AT7587724</v>
       </c>
       <c r="H36">
-        <f>_xll.BDH(G36&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>104.721</v>
+        <f>_xll.BDH(G36&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>104.59</v>
       </c>
       <c r="I36">
-        <v>104.72199999999999</v>
+        <v>104.66</v>
       </c>
       <c r="J36">
-        <v>104.57299999999999</v>
+        <v>104.59</v>
       </c>
       <c r="K36">
-        <v>104.744</v>
+        <v>104.67</v>
       </c>
       <c r="L36">
-        <v>104.254</v>
+        <v>104.43</v>
       </c>
       <c r="M36">
-        <v>104.036</v>
+        <v>103.97</v>
       </c>
       <c r="N36">
-        <v>103.352</v>
+        <v>103.64</v>
       </c>
       <c r="O36">
-        <v>103.407</v>
+        <v>103.51</v>
       </c>
       <c r="P36">
-        <v>103.69</v>
+        <v>103.51</v>
       </c>
       <c r="Q36">
-        <v>104.01600000000001</v>
+        <v>104.02</v>
       </c>
       <c r="R36">
-        <v>103.89700000000001</v>
+        <v>104.35</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -5396,38 +5396,38 @@
         <v>AZ8014799</v>
       </c>
       <c r="H37">
-        <f>_xll.BDH(G37&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>97.031999999999996</v>
+        <f>_xll.BDH(G37&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>96.7</v>
       </c>
       <c r="I37">
-        <v>97.043000000000006</v>
+        <v>96.91</v>
       </c>
       <c r="J37">
-        <v>96.899000000000001</v>
+        <v>96.98</v>
       </c>
       <c r="K37">
-        <v>97.108000000000004</v>
+        <v>96.96</v>
       </c>
       <c r="L37">
-        <v>96.570999999999998</v>
+        <v>96.76</v>
       </c>
       <c r="M37">
-        <v>96.361000000000004</v>
+        <v>96.28</v>
       </c>
       <c r="N37">
-        <v>95.644999999999996</v>
+        <v>95.98</v>
       </c>
       <c r="O37">
-        <v>95.747</v>
+        <v>95.73</v>
       </c>
       <c r="P37">
-        <v>96.066999999999993</v>
+        <v>95.9</v>
       </c>
       <c r="Q37">
-        <v>96.409000000000006</v>
+        <v>96.46</v>
       </c>
       <c r="R37">
-        <v>96.265000000000001</v>
+        <v>96.75</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -5459,38 +5459,38 @@
         <v>ZO7604374</v>
       </c>
       <c r="H38">
-        <f>_xll.BDH(G38&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>90.349000000000004</v>
+        <f>_xll.BDH(G38&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>90.22</v>
       </c>
       <c r="I38">
-        <v>90.367999999999995</v>
+        <v>90.3</v>
       </c>
       <c r="J38">
-        <v>90.212000000000003</v>
+        <v>90.24</v>
       </c>
       <c r="K38">
-        <v>90.438999999999993</v>
+        <v>90.34</v>
       </c>
       <c r="L38">
-        <v>89.894999999999996</v>
+        <v>90.09</v>
       </c>
       <c r="M38">
-        <v>89.677000000000007</v>
+        <v>89.59</v>
       </c>
       <c r="N38">
-        <v>88.97</v>
+        <v>89.28</v>
       </c>
       <c r="O38">
-        <v>89.07</v>
+        <v>89.17</v>
       </c>
       <c r="P38">
-        <v>89.402000000000001</v>
+        <v>89.18</v>
       </c>
       <c r="Q38">
-        <v>89.753</v>
+        <v>89.75</v>
       </c>
       <c r="R38">
-        <v>89.602000000000004</v>
+        <v>90.13</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -5522,38 +5522,38 @@
         <v>BP2380833</v>
       </c>
       <c r="H39">
-        <f>_xll.BDH(G39&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>98.177000000000007</v>
+        <f>_xll.BDH(G39&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>98.02</v>
       </c>
       <c r="I39">
-        <v>98.197999999999993</v>
+        <v>98.13</v>
       </c>
       <c r="J39">
-        <v>98.02</v>
+        <v>98.03</v>
       </c>
       <c r="K39">
-        <v>98.254999999999995</v>
+        <v>98.14</v>
       </c>
       <c r="L39">
-        <v>97.667000000000002</v>
+        <v>97.87</v>
       </c>
       <c r="M39">
-        <v>97.438999999999993</v>
+        <v>97.33</v>
       </c>
       <c r="N39">
-        <v>96.665000000000006</v>
+        <v>96.99</v>
       </c>
       <c r="O39">
-        <v>96.787000000000006</v>
+        <v>96.88</v>
       </c>
       <c r="P39">
-        <v>97.14</v>
+        <v>96.99</v>
       </c>
       <c r="Q39">
-        <v>97.522000000000006</v>
+        <v>97.51</v>
       </c>
       <c r="R39">
-        <v>97.349000000000004</v>
+        <v>97.91</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -5585,38 +5585,38 @@
         <v>BS0709235</v>
       </c>
       <c r="H40">
-        <f>_xll.BDH(G40&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD","cols=11;rows=1")</f>
-        <v>97.596000000000004</v>
+        <f>_xll.BDH(G40&amp;" GF Corp", "PX_LAST", "1/10/2022", "1/24/2022", "Dates", "H", "Direction", "H", "Currency", "CAD", "PCS", "FRNK","cols=11;rows=1")</f>
+        <v>97.43</v>
       </c>
       <c r="I40">
-        <v>97.613</v>
+        <v>97.53</v>
       </c>
       <c r="J40">
-        <v>97.423000000000002</v>
+        <v>97.43</v>
       </c>
       <c r="K40">
-        <v>97.676000000000002</v>
+        <v>97.54</v>
       </c>
       <c r="L40">
-        <v>97.072000000000003</v>
+        <v>97.28</v>
       </c>
       <c r="M40">
-        <v>96.831000000000003</v>
+        <v>96.71</v>
       </c>
       <c r="N40">
-        <v>96.037999999999997</v>
+        <v>96.37</v>
       </c>
       <c r="O40">
-        <v>96.173000000000002</v>
+        <v>96.27</v>
       </c>
       <c r="P40">
-        <v>96.555999999999997</v>
+        <v>96.39</v>
       </c>
       <c r="Q40">
-        <v>96.956000000000003</v>
+        <v>96.94</v>
       </c>
       <c r="R40">
-        <v>96.775000000000006</v>
+        <v>97.36</v>
       </c>
     </row>
   </sheetData>
@@ -5629,42 +5629,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1">
@@ -5724,37 +5725,37 @@
         <v>31</v>
       </c>
       <c r="H2">
-        <v>100.068</v>
+        <v>100.065</v>
       </c>
       <c r="I2">
-        <v>100.06399999999999</v>
+        <v>100.062</v>
       </c>
       <c r="J2">
-        <v>100.06</v>
+        <v>100.057</v>
       </c>
       <c r="K2">
-        <v>100.047</v>
+        <v>100.04600000000001</v>
       </c>
       <c r="L2">
-        <v>100.044</v>
+        <v>100.042</v>
       </c>
       <c r="M2">
-        <v>100.038</v>
+        <v>100.035</v>
       </c>
       <c r="N2">
-        <v>100.03400000000001</v>
+        <v>100.03</v>
       </c>
       <c r="O2">
-        <v>100.03</v>
+        <v>100.027</v>
       </c>
       <c r="P2">
-        <v>100.02200000000001</v>
+        <v>100.02</v>
       </c>
       <c r="Q2">
-        <v>100.01900000000001</v>
+        <v>100.032</v>
       </c>
       <c r="R2">
-        <v>100.01600000000001</v>
+        <v>100.014</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5780,37 +5781,37 @@
         <v>35</v>
       </c>
       <c r="H3">
-        <v>100.04300000000001</v>
+        <v>100.038</v>
       </c>
       <c r="I3">
-        <v>100.042</v>
+        <v>100.036</v>
       </c>
       <c r="J3">
-        <v>100.035</v>
+        <v>100.032</v>
       </c>
       <c r="K3">
-        <v>100.03</v>
+        <v>100.02800000000001</v>
       </c>
       <c r="L3">
-        <v>100.027</v>
+        <v>100.02500000000001</v>
       </c>
       <c r="M3">
-        <v>100.01900000000001</v>
+        <v>100.015</v>
       </c>
       <c r="N3">
+        <v>100.01</v>
+      </c>
+      <c r="O3">
+        <v>100.011</v>
+      </c>
+      <c r="P3">
+        <v>100.011</v>
+      </c>
+      <c r="Q3">
         <v>100.014</v>
       </c>
-      <c r="O3">
-        <v>100.014</v>
-      </c>
-      <c r="P3">
+      <c r="R3">
         <v>100.01600000000001</v>
-      </c>
-      <c r="Q3">
-        <v>100.017</v>
-      </c>
-      <c r="R3">
-        <v>100.018</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -5836,37 +5837,37 @@
         <v>39</v>
       </c>
       <c r="H4">
-        <v>100.351</v>
+        <v>100.349</v>
       </c>
       <c r="I4">
-        <v>100.346</v>
+        <v>100.34099999999999</v>
       </c>
       <c r="J4">
-        <v>100.33199999999999</v>
+        <v>100.333</v>
       </c>
       <c r="K4">
-        <v>100.322</v>
+        <v>100.32</v>
       </c>
       <c r="L4">
-        <v>100.306</v>
+        <v>100.309</v>
       </c>
       <c r="M4">
-        <v>100.288</v>
+        <v>100.28400000000001</v>
       </c>
       <c r="N4">
         <v>100.26900000000001</v>
       </c>
       <c r="O4">
-        <v>100.268</v>
+        <v>100.26600000000001</v>
       </c>
       <c r="P4">
+        <v>100.261</v>
+      </c>
+      <c r="Q4">
         <v>100.26900000000001</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>100.27</v>
-      </c>
-      <c r="R4">
-        <v>100.26900000000001</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -5892,37 +5893,37 @@
         <v>43</v>
       </c>
       <c r="H5">
-        <v>100.90600000000001</v>
+        <v>100.75700000000001</v>
       </c>
       <c r="I5">
-        <v>100.899</v>
+        <v>100.742</v>
       </c>
       <c r="J5">
-        <v>100.875</v>
+        <v>100.73399999999999</v>
       </c>
       <c r="K5">
-        <v>100.857</v>
+        <v>100.702</v>
       </c>
       <c r="L5">
-        <v>100.834</v>
+        <v>100.68899999999999</v>
       </c>
       <c r="M5">
-        <v>100.806</v>
+        <v>100.651</v>
       </c>
       <c r="N5">
-        <v>100.78</v>
+        <v>100.64</v>
       </c>
       <c r="O5">
-        <v>100.779</v>
+        <v>100.617</v>
       </c>
       <c r="P5">
-        <v>100.77200000000001</v>
+        <v>100.613</v>
       </c>
       <c r="Q5">
-        <v>100.77200000000001</v>
+        <v>100.627</v>
       </c>
       <c r="R5">
-        <v>100.767</v>
+        <v>100.621</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -5948,37 +5949,37 @@
         <v>46</v>
       </c>
       <c r="H6">
-        <v>103.407</v>
+        <v>103.395</v>
       </c>
       <c r="I6">
-        <v>103.38500000000001</v>
+        <v>103.36499999999999</v>
       </c>
       <c r="J6">
-        <v>103.333</v>
+        <v>103.334</v>
       </c>
       <c r="K6">
-        <v>103.27200000000001</v>
+        <v>103.256</v>
       </c>
       <c r="L6">
-        <v>103.22499999999999</v>
+        <v>103.221</v>
       </c>
       <c r="M6">
-        <v>103.18600000000001</v>
+        <v>103.16800000000001</v>
       </c>
       <c r="N6">
-        <v>103.13500000000001</v>
+        <v>103.13</v>
       </c>
       <c r="O6">
-        <v>103.117</v>
+        <v>103.105</v>
       </c>
       <c r="P6">
-        <v>103.053</v>
+        <v>103.038</v>
       </c>
       <c r="Q6">
-        <v>103.035</v>
+        <v>103.02800000000001</v>
       </c>
       <c r="R6">
-        <v>103.021</v>
+        <v>103.011</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -6004,37 +6005,37 @@
         <v>50</v>
       </c>
       <c r="H7">
-        <v>99.796999999999997</v>
+        <v>99.793999999999997</v>
       </c>
       <c r="I7">
-        <v>99.8</v>
+        <v>99.786000000000001</v>
       </c>
       <c r="J7">
-        <v>99.772000000000006</v>
+        <v>99.775999999999996</v>
       </c>
       <c r="K7">
-        <v>99.774000000000001</v>
+        <v>99.77</v>
       </c>
       <c r="L7">
-        <v>99.754999999999995</v>
+        <v>99.759</v>
       </c>
       <c r="M7">
-        <v>99.724000000000004</v>
+        <v>99.718999999999994</v>
       </c>
       <c r="N7">
-        <v>99.694999999999993</v>
+        <v>99.697000000000003</v>
       </c>
       <c r="O7">
-        <v>99.703000000000003</v>
+        <v>99.700999999999993</v>
       </c>
       <c r="P7">
-        <v>99.724999999999994</v>
+        <v>99.713999999999999</v>
       </c>
       <c r="Q7">
-        <v>99.741</v>
+        <v>99.739000000000004</v>
       </c>
       <c r="R7">
-        <v>99.745999999999995</v>
+        <v>99.748000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -6060,37 +6061,37 @@
         <v>54</v>
       </c>
       <c r="H8">
-        <v>100.197</v>
+        <v>100.19799999999999</v>
       </c>
       <c r="I8">
-        <v>100.196</v>
+        <v>100.187</v>
       </c>
       <c r="J8">
-        <v>100.16800000000001</v>
+        <v>100.17400000000001</v>
       </c>
       <c r="K8">
-        <v>100.166</v>
+        <v>100.16200000000001</v>
       </c>
       <c r="L8">
-        <v>100.134</v>
+        <v>100.145</v>
       </c>
       <c r="M8">
-        <v>100.1</v>
+        <v>100.09399999999999</v>
       </c>
       <c r="N8">
-        <v>100.066</v>
+        <v>100.069</v>
       </c>
       <c r="O8">
-        <v>100.074</v>
+        <v>100.071</v>
       </c>
       <c r="P8">
-        <v>100.09399999999999</v>
+        <v>100.081</v>
       </c>
       <c r="Q8">
-        <v>100.108</v>
+        <v>100.105</v>
       </c>
       <c r="R8">
-        <v>100.108</v>
+        <v>100.114</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -6116,37 +6117,37 @@
         <v>58</v>
       </c>
       <c r="H9">
-        <v>99.551000000000002</v>
+        <v>99.552000000000007</v>
       </c>
       <c r="I9">
-        <v>99.554000000000002</v>
+        <v>99.540999999999997</v>
       </c>
       <c r="J9">
+        <v>99.527000000000001</v>
+      </c>
+      <c r="K9">
         <v>99.52</v>
       </c>
-      <c r="K9">
-        <v>99.525999999999996</v>
-      </c>
       <c r="L9">
-        <v>99.488</v>
+        <v>99.501000000000005</v>
       </c>
       <c r="M9">
-        <v>99.447999999999993</v>
+        <v>99.438999999999993</v>
       </c>
       <c r="N9">
-        <v>99.408000000000001</v>
+        <v>99.409000000000006</v>
       </c>
       <c r="O9">
         <v>99.415999999999997</v>
       </c>
       <c r="P9">
-        <v>99.448999999999998</v>
+        <v>99.432000000000002</v>
       </c>
       <c r="Q9">
-        <v>99.468000000000004</v>
+        <v>99.47</v>
       </c>
       <c r="R9">
-        <v>99.475999999999999</v>
+        <v>99.483999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -6172,37 +6173,37 @@
         <v>62</v>
       </c>
       <c r="H10">
-        <v>99.316000000000003</v>
+        <v>99.307000000000002</v>
       </c>
       <c r="I10">
-        <v>99.320999999999998</v>
+        <v>99.301000000000002</v>
       </c>
       <c r="J10">
-        <v>99.278999999999996</v>
+        <v>99.281999999999996</v>
       </c>
       <c r="K10">
-        <v>99.284000000000006</v>
+        <v>99.274000000000001</v>
       </c>
       <c r="L10">
-        <v>99.233000000000004</v>
+        <v>99.251000000000005</v>
       </c>
       <c r="M10">
-        <v>99.179000000000002</v>
+        <v>99.17</v>
       </c>
       <c r="N10">
-        <v>99.125</v>
+        <v>99.132000000000005</v>
       </c>
       <c r="O10">
-        <v>99.132000000000005</v>
+        <v>99.14</v>
       </c>
       <c r="P10">
-        <v>99.168999999999997</v>
+        <v>99.156000000000006</v>
       </c>
       <c r="Q10">
-        <v>99.194999999999993</v>
+        <v>99.206000000000003</v>
       </c>
       <c r="R10">
-        <v>99.206000000000003</v>
+        <v>99.221999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -6228,37 +6229,37 @@
         <v>66</v>
       </c>
       <c r="H11">
-        <v>100.944</v>
+        <v>100.934</v>
       </c>
       <c r="I11">
-        <v>100.94199999999999</v>
+        <v>100.92100000000001</v>
       </c>
       <c r="J11">
-        <v>100.887</v>
+        <v>100.9</v>
       </c>
       <c r="K11">
-        <v>100.884</v>
+        <v>100.874</v>
       </c>
       <c r="L11">
-        <v>100.83199999999999</v>
+        <v>100.85299999999999</v>
       </c>
       <c r="M11">
-        <v>100.764</v>
+        <v>100.755</v>
       </c>
       <c r="N11">
-        <v>100.70699999999999</v>
+        <v>100.71</v>
       </c>
       <c r="O11">
-        <v>100.699</v>
+        <v>100.711</v>
       </c>
       <c r="P11">
-        <v>100.718</v>
+        <v>100.709</v>
       </c>
       <c r="Q11">
-        <v>100.739</v>
+        <v>100.748</v>
       </c>
       <c r="R11">
-        <v>100.746</v>
+        <v>100.76600000000001</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -6284,37 +6285,37 @@
         <v>70</v>
       </c>
       <c r="H12">
-        <v>99.09</v>
+        <v>99.081999999999994</v>
       </c>
       <c r="I12">
-        <v>99.094999999999999</v>
+        <v>99.073999999999998</v>
       </c>
       <c r="J12">
-        <v>99.043999999999997</v>
+        <v>99.055999999999997</v>
       </c>
       <c r="K12">
-        <v>99.054000000000002</v>
+        <v>99.042000000000002</v>
       </c>
       <c r="L12">
-        <v>98.991</v>
+        <v>99.018000000000001</v>
       </c>
       <c r="M12">
-        <v>98.923000000000002</v>
+        <v>98.912999999999997</v>
       </c>
       <c r="N12">
-        <v>98.855000000000004</v>
+        <v>98.864000000000004</v>
       </c>
       <c r="O12">
-        <v>98.858999999999995</v>
+        <v>98.873999999999995</v>
       </c>
       <c r="P12">
-        <v>98.888999999999996</v>
+        <v>98.882999999999996</v>
       </c>
       <c r="Q12">
-        <v>98.918000000000006</v>
+        <v>98.93</v>
       </c>
       <c r="R12">
-        <v>98.923000000000002</v>
+        <v>98.954999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -6340,37 +6341,37 @@
         <v>74</v>
       </c>
       <c r="H13">
-        <v>109.66</v>
+        <v>109.629</v>
       </c>
       <c r="I13">
-        <v>109.655</v>
+        <v>109.592</v>
       </c>
       <c r="J13">
-        <v>109.556</v>
+        <v>109.548</v>
       </c>
       <c r="K13">
-        <v>109.506</v>
+        <v>109.46899999999999</v>
       </c>
       <c r="L13">
-        <v>109.417</v>
+        <v>109.42100000000001</v>
       </c>
       <c r="M13">
-        <v>109.319</v>
+        <v>109.27800000000001</v>
       </c>
       <c r="N13">
-        <v>109.21899999999999</v>
+        <v>109.20099999999999</v>
       </c>
       <c r="O13">
-        <v>109.197</v>
+        <v>109.18899999999999</v>
       </c>
       <c r="P13">
-        <v>109.16200000000001</v>
+        <v>109.13200000000001</v>
       </c>
       <c r="Q13">
-        <v>109.17</v>
+        <v>109.161</v>
       </c>
       <c r="R13">
-        <v>109.173</v>
+        <v>109.169</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -6396,37 +6397,37 @@
         <v>77</v>
       </c>
       <c r="H14">
-        <v>100.727</v>
+        <v>100.70699999999999</v>
       </c>
       <c r="I14">
-        <v>100.723</v>
+        <v>100.687</v>
       </c>
       <c r="J14">
-        <v>100.663</v>
+        <v>100.678</v>
       </c>
       <c r="K14">
-        <v>100.66500000000001</v>
+        <v>100.637</v>
       </c>
       <c r="L14">
-        <v>100.593</v>
+        <v>100.6</v>
       </c>
       <c r="M14">
-        <v>100.514</v>
+        <v>100.485</v>
       </c>
       <c r="N14">
-        <v>100.437</v>
+        <v>100.432</v>
       </c>
       <c r="O14">
-        <v>100.437</v>
+        <v>100.43600000000001</v>
       </c>
       <c r="P14">
-        <v>100.45699999999999</v>
+        <v>100.443</v>
       </c>
       <c r="Q14">
-        <v>100.48099999999999</v>
+        <v>100.488</v>
       </c>
       <c r="R14">
-        <v>100.48699999999999</v>
+        <v>100.505</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -6452,37 +6453,37 @@
         <v>81</v>
       </c>
       <c r="H15">
-        <v>98.820999999999998</v>
+        <v>98.808000000000007</v>
       </c>
       <c r="I15">
-        <v>98.822000000000003</v>
+        <v>98.8</v>
       </c>
       <c r="J15">
-        <v>98.762</v>
+        <v>98.781000000000006</v>
       </c>
       <c r="K15">
-        <v>98.778000000000006</v>
+        <v>98.763000000000005</v>
       </c>
       <c r="L15">
-        <v>98.7</v>
+        <v>98.736000000000004</v>
       </c>
       <c r="M15">
-        <v>98.619</v>
+        <v>98.61</v>
       </c>
       <c r="N15">
-        <v>98.534999999999997</v>
+        <v>98.552999999999997</v>
       </c>
       <c r="O15">
-        <v>98.534000000000006</v>
+        <v>98.549000000000007</v>
       </c>
       <c r="P15">
-        <v>98.563999999999993</v>
+        <v>98.558000000000007</v>
       </c>
       <c r="Q15">
-        <v>98.6</v>
+        <v>98.611000000000004</v>
       </c>
       <c r="R15">
-        <v>98.605999999999995</v>
+        <v>98.635000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -6508,37 +6509,37 @@
         <v>85</v>
       </c>
       <c r="H16">
-        <v>101.574</v>
+        <v>101.565</v>
       </c>
       <c r="I16">
-        <v>101.57299999999999</v>
+        <v>101.548</v>
       </c>
       <c r="J16">
-        <v>101.504</v>
+        <v>101.523</v>
       </c>
       <c r="K16">
-        <v>101.509</v>
+        <v>101.492</v>
       </c>
       <c r="L16">
-        <v>101.42100000000001</v>
+        <v>101.459</v>
       </c>
       <c r="M16">
-        <v>101.32599999999999</v>
+        <v>101.319</v>
       </c>
       <c r="N16">
-        <v>101.23</v>
+        <v>101.254</v>
       </c>
       <c r="O16">
-        <v>101.226</v>
+        <v>101.241</v>
       </c>
       <c r="P16">
-        <v>101.24299999999999</v>
+        <v>101.233</v>
       </c>
       <c r="Q16">
-        <v>101.268</v>
+        <v>101.286</v>
       </c>
       <c r="R16">
-        <v>101.271</v>
+        <v>101.30800000000001</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -6564,37 +6565,37 @@
         <v>89</v>
       </c>
       <c r="H17">
-        <v>98.978999999999999</v>
+        <v>98.968000000000004</v>
       </c>
       <c r="I17">
-        <v>98.981999999999999</v>
+        <v>98.954999999999998</v>
       </c>
       <c r="J17">
+        <v>98.933999999999997</v>
+      </c>
+      <c r="K17">
         <v>98.911000000000001</v>
       </c>
-      <c r="K17">
-        <v>98.926000000000002</v>
-      </c>
       <c r="L17">
-        <v>98.835999999999999</v>
+        <v>98.878</v>
       </c>
       <c r="M17">
-        <v>98.742000000000004</v>
+        <v>98.731999999999999</v>
       </c>
       <c r="N17">
-        <v>98.64</v>
+        <v>98.665999999999997</v>
       </c>
       <c r="O17">
-        <v>98.638999999999996</v>
+        <v>98.653999999999996</v>
       </c>
       <c r="P17">
-        <v>98.668999999999997</v>
+        <v>98.661000000000001</v>
       </c>
       <c r="Q17">
-        <v>98.698999999999998</v>
+        <v>98.716999999999999</v>
       </c>
       <c r="R17">
-        <v>98.710999999999999</v>
+        <v>98.745999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -6620,37 +6621,37 @@
         <v>93</v>
       </c>
       <c r="H18">
-        <v>99.224000000000004</v>
+        <v>99.21</v>
       </c>
       <c r="I18">
-        <v>99.216999999999999</v>
+        <v>99.19</v>
       </c>
       <c r="J18">
-        <v>99.134</v>
+        <v>99.165000000000006</v>
       </c>
       <c r="K18">
-        <v>99.143000000000001</v>
+        <v>99.13</v>
       </c>
       <c r="L18">
-        <v>99.036000000000001</v>
+        <v>99.09</v>
       </c>
       <c r="M18">
-        <v>98.930999999999997</v>
+        <v>98.92</v>
       </c>
       <c r="N18">
-        <v>98.820999999999998</v>
+        <v>98.844999999999999</v>
       </c>
       <c r="O18">
-        <v>98.817999999999998</v>
+        <v>98.84</v>
       </c>
       <c r="P18">
-        <v>98.855000000000004</v>
+        <v>98.844999999999999</v>
       </c>
       <c r="Q18">
-        <v>98.903999999999996</v>
+        <v>98.92</v>
       </c>
       <c r="R18">
-        <v>98.915999999999997</v>
+        <v>98.954999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -6676,37 +6677,37 @@
         <v>97</v>
       </c>
       <c r="H19">
-        <v>102.34</v>
+        <v>102.32</v>
       </c>
       <c r="I19">
-        <v>102.331</v>
+        <v>102.29</v>
       </c>
       <c r="J19">
-        <v>102.238</v>
+        <v>102.28</v>
       </c>
       <c r="K19">
-        <v>102.242</v>
+        <v>102.23</v>
       </c>
       <c r="L19">
-        <v>102.126</v>
+        <v>102.18</v>
       </c>
       <c r="M19">
-        <v>102.008</v>
+        <v>102</v>
       </c>
       <c r="N19">
-        <v>101.883</v>
+        <v>101.91</v>
       </c>
       <c r="O19">
-        <v>101.877</v>
+        <v>101.89</v>
       </c>
       <c r="P19">
-        <v>101.901</v>
+        <v>101.89</v>
       </c>
       <c r="Q19">
-        <v>101.949</v>
+        <v>101.985</v>
       </c>
       <c r="R19">
-        <v>101.95099999999999</v>
+        <v>101.985</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -6732,37 +6733,37 @@
         <v>101</v>
       </c>
       <c r="H20">
-        <v>97.997</v>
+        <v>97.974999999999994</v>
       </c>
       <c r="I20">
-        <v>97.992999999999995</v>
+        <v>97.96</v>
       </c>
       <c r="J20">
+        <v>97.93</v>
+      </c>
+      <c r="K20">
         <v>97.905000000000001</v>
       </c>
-      <c r="K20">
-        <v>97.927000000000007</v>
-      </c>
       <c r="L20">
-        <v>97.811000000000007</v>
+        <v>97.864999999999995</v>
       </c>
       <c r="M20">
-        <v>97.697999999999993</v>
+        <v>97.674999999999997</v>
       </c>
       <c r="N20">
-        <v>97.581000000000003</v>
+        <v>97.61</v>
       </c>
       <c r="O20">
-        <v>97.584000000000003</v>
+        <v>97.594999999999999</v>
       </c>
       <c r="P20">
-        <v>97.64</v>
+        <v>97.61</v>
       </c>
       <c r="Q20">
-        <v>97.695999999999998</v>
+        <v>97.715000000000003</v>
       </c>
       <c r="R20">
-        <v>97.712999999999994</v>
+        <v>97.754999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -6788,37 +6789,37 @@
         <v>105</v>
       </c>
       <c r="H21">
-        <v>103.048</v>
+        <v>102.925</v>
       </c>
       <c r="I21">
-        <v>103.047</v>
+        <v>102.86</v>
       </c>
       <c r="J21">
-        <v>102.947</v>
+        <v>102.85</v>
       </c>
       <c r="K21">
-        <v>102.953</v>
+        <v>102.8</v>
       </c>
       <c r="L21">
-        <v>102.82</v>
+        <v>102.78</v>
       </c>
       <c r="M21">
-        <v>102.691</v>
+        <v>102.55500000000001</v>
       </c>
       <c r="N21">
-        <v>102.56399999999999</v>
+        <v>102.485</v>
       </c>
       <c r="O21">
-        <v>102.56399999999999</v>
+        <v>102.42</v>
       </c>
       <c r="P21">
-        <v>102.602</v>
+        <v>102.45</v>
       </c>
       <c r="Q21">
-        <v>102.65600000000001</v>
+        <v>102.53</v>
       </c>
       <c r="R21">
-        <v>102.666</v>
+        <v>102.61499999999999</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -6844,37 +6845,37 @@
         <v>109</v>
       </c>
       <c r="H22">
-        <v>100.69</v>
+        <v>100.55</v>
       </c>
       <c r="I22">
-        <v>100.697</v>
+        <v>100.52</v>
       </c>
       <c r="J22">
-        <v>100.59399999999999</v>
+        <v>100.56</v>
       </c>
       <c r="K22">
-        <v>100.599</v>
+        <v>100.45</v>
       </c>
       <c r="L22">
-        <v>100.458</v>
+        <v>100.44</v>
       </c>
       <c r="M22">
-        <v>100.31399999999999</v>
+        <v>100.32</v>
       </c>
       <c r="N22">
-        <v>100.181</v>
+        <v>100.14</v>
       </c>
       <c r="O22">
-        <v>100.173</v>
+        <v>100.02</v>
       </c>
       <c r="P22">
-        <v>100.241</v>
+        <v>100.04</v>
       </c>
       <c r="Q22">
-        <v>100.313</v>
+        <v>100.11</v>
       </c>
       <c r="R22">
-        <v>100.334</v>
+        <v>100.18</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -6900,37 +6901,37 @@
         <v>113</v>
       </c>
       <c r="H23">
-        <v>98.59</v>
+        <v>98.56</v>
       </c>
       <c r="I23">
-        <v>98.591999999999999</v>
+        <v>98.555000000000007</v>
       </c>
       <c r="J23">
-        <v>98.489000000000004</v>
+        <v>98.53</v>
       </c>
       <c r="K23">
-        <v>98.516000000000005</v>
+        <v>98.484999999999999</v>
       </c>
       <c r="L23">
-        <v>98.367999999999995</v>
+        <v>98.435000000000002</v>
       </c>
       <c r="M23">
-        <v>98.23</v>
+        <v>98.21</v>
       </c>
       <c r="N23">
-        <v>98.082999999999998</v>
+        <v>98.13</v>
       </c>
       <c r="O23">
-        <v>98.100999999999999</v>
+        <v>98.11</v>
       </c>
       <c r="P23">
-        <v>98.192999999999998</v>
+        <v>98.15</v>
       </c>
       <c r="Q23">
-        <v>98.289000000000001</v>
+        <v>98.29</v>
       </c>
       <c r="R23">
-        <v>98.302000000000007</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -6956,37 +6957,37 @@
         <v>117</v>
       </c>
       <c r="H24">
-        <v>99.715999999999994</v>
+        <v>99.65</v>
       </c>
       <c r="I24">
-        <v>99.716999999999999</v>
+        <v>99.655000000000001</v>
       </c>
       <c r="J24">
-        <v>99.602999999999994</v>
+        <v>99.614999999999995</v>
       </c>
       <c r="K24">
-        <v>99.646000000000001</v>
+        <v>99.584999999999994</v>
       </c>
       <c r="L24">
-        <v>99.456000000000003</v>
+        <v>99.5</v>
       </c>
       <c r="M24">
-        <v>99.302000000000007</v>
+        <v>99.254999999999995</v>
       </c>
       <c r="N24">
-        <v>99.113</v>
+        <v>99.125</v>
       </c>
       <c r="O24">
-        <v>99.108999999999995</v>
+        <v>99.105000000000004</v>
       </c>
       <c r="P24">
-        <v>99.192999999999998</v>
+        <v>99.12</v>
       </c>
       <c r="Q24">
-        <v>99.29</v>
+        <v>99.284999999999997</v>
       </c>
       <c r="R24">
-        <v>99.34</v>
+        <v>99.37</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -7012,37 +7013,37 @@
         <v>121</v>
       </c>
       <c r="H25">
-        <v>125.22499999999999</v>
+        <v>125.08</v>
       </c>
       <c r="I25">
-        <v>125.21899999999999</v>
+        <v>125.1</v>
       </c>
       <c r="J25">
-        <v>125.044</v>
+        <v>125.07</v>
       </c>
       <c r="K25">
-        <v>125.068</v>
+        <v>125.03</v>
       </c>
       <c r="L25">
-        <v>124.837</v>
+        <v>124.9</v>
       </c>
       <c r="M25">
-        <v>124.636</v>
+        <v>124.57</v>
       </c>
       <c r="N25">
-        <v>124.26600000000001</v>
+        <v>124.37</v>
       </c>
       <c r="O25">
-        <v>124.264</v>
+        <v>124.28</v>
       </c>
       <c r="P25">
-        <v>124.277</v>
+        <v>124.2</v>
       </c>
       <c r="Q25">
-        <v>124.393</v>
+        <v>124.39</v>
       </c>
       <c r="R25">
-        <v>124.376</v>
+        <v>124.51</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -7068,37 +7069,37 @@
         <v>124</v>
       </c>
       <c r="H26">
-        <v>102.979</v>
+        <v>102.92</v>
       </c>
       <c r="I26">
-        <v>102.99</v>
+        <v>102.95</v>
       </c>
       <c r="J26">
-        <v>102.866</v>
+        <v>102.905</v>
       </c>
       <c r="K26">
-        <v>102.93300000000001</v>
+        <v>102.905</v>
       </c>
       <c r="L26">
-        <v>102.741</v>
+        <v>102.81</v>
       </c>
       <c r="M26">
-        <v>102.557</v>
+        <v>102.535</v>
       </c>
       <c r="N26">
-        <v>102.268</v>
+        <v>102.355</v>
       </c>
       <c r="O26">
-        <v>102.252</v>
+        <v>102.30500000000001</v>
       </c>
       <c r="P26">
-        <v>102.33199999999999</v>
+        <v>102.295</v>
       </c>
       <c r="Q26">
-        <v>102.453</v>
+        <v>102.47</v>
       </c>
       <c r="R26">
-        <v>102.429</v>
+        <v>102.58</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -7124,37 +7125,37 @@
         <v>128</v>
       </c>
       <c r="H27">
-        <v>96.826999999999998</v>
+        <v>96.704999999999998</v>
       </c>
       <c r="I27">
-        <v>96.837999999999994</v>
+        <v>96.74</v>
       </c>
       <c r="J27">
-        <v>96.718000000000004</v>
+        <v>96.72</v>
       </c>
       <c r="K27">
-        <v>96.81</v>
+        <v>96.734999999999999</v>
       </c>
       <c r="L27">
-        <v>96.603999999999999</v>
+        <v>96.68</v>
       </c>
       <c r="M27">
-        <v>96.47</v>
+        <v>96.41</v>
       </c>
       <c r="N27">
-        <v>96.14</v>
+        <v>96.25</v>
       </c>
       <c r="O27">
-        <v>96.150999999999996</v>
+        <v>96.144999999999996</v>
       </c>
       <c r="P27">
-        <v>96.251000000000005</v>
+        <v>96.174999999999997</v>
       </c>
       <c r="Q27">
-        <v>96.369</v>
+        <v>96.334999999999994</v>
       </c>
       <c r="R27">
-        <v>96.346000000000004</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -7180,37 +7181,37 @@
         <v>132</v>
       </c>
       <c r="H28">
-        <v>95.188999999999993</v>
+        <v>95.114999999999995</v>
       </c>
       <c r="I28">
-        <v>95.203999999999994</v>
+        <v>95.155000000000001</v>
       </c>
       <c r="J28">
-        <v>95.08</v>
+        <v>95.125</v>
       </c>
       <c r="K28">
-        <v>95.177999999999997</v>
+        <v>95.155000000000001</v>
       </c>
       <c r="L28">
-        <v>94.962000000000003</v>
+        <v>95.055000000000007</v>
       </c>
       <c r="M28">
-        <v>94.796999999999997</v>
+        <v>94.754999999999995</v>
       </c>
       <c r="N28">
-        <v>94.444999999999993</v>
+        <v>94.555000000000007</v>
       </c>
       <c r="O28">
-        <v>94.459000000000003</v>
+        <v>94.504999999999995</v>
       </c>
       <c r="P28">
-        <v>94.573999999999998</v>
+        <v>94.545000000000002</v>
       </c>
       <c r="Q28">
-        <v>94.712999999999994</v>
+        <v>94.73</v>
       </c>
       <c r="R28">
-        <v>94.691000000000003</v>
+        <v>94.875</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -7236,37 +7237,37 @@
         <v>136</v>
       </c>
       <c r="H29">
-        <v>100.214</v>
+        <v>100.13500000000001</v>
       </c>
       <c r="I29">
-        <v>100.221</v>
+        <v>100.175</v>
       </c>
       <c r="J29">
-        <v>100.089</v>
+        <v>100.14</v>
       </c>
       <c r="K29">
-        <v>100.19</v>
+        <v>100.155</v>
       </c>
       <c r="L29">
-        <v>99.947000000000003</v>
+        <v>100.04</v>
       </c>
       <c r="M29">
-        <v>99.763999999999996</v>
+        <v>99.71</v>
       </c>
       <c r="N29">
-        <v>99.375</v>
+        <v>99.545000000000002</v>
       </c>
       <c r="O29">
-        <v>99.387</v>
+        <v>99.435000000000002</v>
       </c>
       <c r="P29">
-        <v>99.503</v>
+        <v>99.44</v>
       </c>
       <c r="Q29">
-        <v>99.653000000000006</v>
+        <v>99.674999999999997</v>
       </c>
       <c r="R29">
-        <v>99.626999999999995</v>
+        <v>99.834999999999994</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -7292,37 +7293,37 @@
         <v>140</v>
       </c>
       <c r="H30">
-        <v>97.75</v>
+        <v>97.66</v>
       </c>
       <c r="I30">
-        <v>97.754000000000005</v>
+        <v>97.7</v>
       </c>
       <c r="J30">
-        <v>97.625</v>
+        <v>97.67</v>
       </c>
       <c r="K30">
-        <v>97.742999999999995</v>
+        <v>97.694999999999993</v>
       </c>
       <c r="L30">
-        <v>97.488</v>
+        <v>97.584999999999994</v>
       </c>
       <c r="M30">
-        <v>97.298000000000002</v>
+        <v>97.24</v>
       </c>
       <c r="N30">
-        <v>96.900999999999996</v>
+        <v>97.02</v>
       </c>
       <c r="O30">
-        <v>96.917000000000002</v>
+        <v>96.96</v>
       </c>
       <c r="P30">
-        <v>97.046000000000006</v>
+        <v>97</v>
       </c>
       <c r="Q30">
-        <v>97.212999999999994</v>
+        <v>97.224999999999994</v>
       </c>
       <c r="R30">
-        <v>97.192999999999998</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -7348,37 +7349,37 @@
         <v>144</v>
       </c>
       <c r="H31">
-        <v>98.5</v>
+        <v>98.41</v>
       </c>
       <c r="I31">
-        <v>98.5</v>
+        <v>98.45</v>
       </c>
       <c r="J31">
-        <v>98.394000000000005</v>
+        <v>98.41</v>
       </c>
       <c r="K31">
-        <v>98.504000000000005</v>
+        <v>98.454999999999998</v>
       </c>
       <c r="L31">
-        <v>98.22</v>
+        <v>98.33</v>
       </c>
       <c r="M31">
-        <v>98.019000000000005</v>
+        <v>97.954999999999998</v>
       </c>
       <c r="N31">
-        <v>97.591999999999999</v>
+        <v>97.715000000000003</v>
       </c>
       <c r="O31">
-        <v>97.628</v>
+        <v>97.665000000000006</v>
       </c>
       <c r="P31">
-        <v>97.760999999999996</v>
+        <v>97.71</v>
       </c>
       <c r="Q31">
-        <v>97.974000000000004</v>
+        <v>97.974999999999994</v>
       </c>
       <c r="R31">
-        <v>97.956999999999994</v>
+        <v>98.185000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -7404,37 +7405,37 @@
         <v>148</v>
       </c>
       <c r="H32">
-        <v>133.434</v>
+        <v>133.285</v>
       </c>
       <c r="I32">
-        <v>133.429</v>
+        <v>133.32</v>
       </c>
       <c r="J32">
-        <v>133.22800000000001</v>
+        <v>133.26</v>
       </c>
       <c r="K32">
-        <v>133.32499999999999</v>
+        <v>133.245</v>
       </c>
       <c r="L32">
-        <v>132.959</v>
+        <v>133.1</v>
       </c>
       <c r="M32">
-        <v>132.68700000000001</v>
+        <v>132.59</v>
       </c>
       <c r="N32">
-        <v>132.12</v>
+        <v>132.27000000000001</v>
       </c>
       <c r="O32">
-        <v>132.124</v>
+        <v>132.16</v>
       </c>
       <c r="P32">
-        <v>132.25399999999999</v>
+        <v>132.13999999999999</v>
       </c>
       <c r="Q32">
-        <v>132.471</v>
+        <v>132.47</v>
       </c>
       <c r="R32">
-        <v>132.41900000000001</v>
+        <v>132.69999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -7460,37 +7461,37 @@
         <v>151</v>
       </c>
       <c r="H33">
-        <v>97.391000000000005</v>
+        <v>97.295000000000002</v>
       </c>
       <c r="I33">
-        <v>97.397000000000006</v>
+        <v>97.34</v>
       </c>
       <c r="J33">
-        <v>97.248999999999995</v>
+        <v>97.305000000000007</v>
       </c>
       <c r="K33">
-        <v>97.381</v>
+        <v>97.334999999999994</v>
       </c>
       <c r="L33">
-        <v>97.09</v>
+        <v>97.21</v>
       </c>
       <c r="M33">
-        <v>96.873000000000005</v>
+        <v>96.814999999999998</v>
       </c>
       <c r="N33">
-        <v>96.418000000000006</v>
+        <v>96.57</v>
       </c>
       <c r="O33">
-        <v>96.432000000000002</v>
+        <v>96.49</v>
       </c>
       <c r="P33">
-        <v>96.584000000000003</v>
+        <v>96.49</v>
       </c>
       <c r="Q33">
-        <v>96.781999999999996</v>
+        <v>96.795000000000002</v>
       </c>
       <c r="R33">
-        <v>96.754999999999995</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -7516,37 +7517,37 @@
         <v>155</v>
       </c>
       <c r="H34">
-        <v>102.72499999999999</v>
+        <v>102.545</v>
       </c>
       <c r="I34">
-        <v>102.699</v>
+        <v>102.595</v>
       </c>
       <c r="J34">
-        <v>102.527</v>
+        <v>102.535</v>
       </c>
       <c r="K34">
-        <v>102.691</v>
+        <v>102.565</v>
       </c>
       <c r="L34">
-        <v>102.321</v>
+        <v>102.42</v>
       </c>
       <c r="M34">
-        <v>102.07299999999999</v>
+        <v>101.94</v>
       </c>
       <c r="N34">
-        <v>101.521</v>
+        <v>101.63500000000001</v>
       </c>
       <c r="O34">
-        <v>101.55200000000001</v>
+        <v>101.55500000000001</v>
       </c>
       <c r="P34">
-        <v>101.756</v>
+        <v>101.63500000000001</v>
       </c>
       <c r="Q34">
-        <v>102.04600000000001</v>
+        <v>102.01</v>
       </c>
       <c r="R34">
-        <v>102.023</v>
+        <v>102.27</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -7572,37 +7573,37 @@
         <v>159</v>
       </c>
       <c r="H35">
-        <v>128.98599999999999</v>
+        <v>128.78</v>
       </c>
       <c r="I35">
-        <v>128.96899999999999</v>
+        <v>128.84</v>
       </c>
       <c r="J35">
-        <v>128.786</v>
+        <v>128.77000000000001</v>
       </c>
       <c r="K35">
-        <v>128.95099999999999</v>
+        <v>128.83000000000001</v>
       </c>
       <c r="L35">
-        <v>128.387</v>
+        <v>128.55000000000001</v>
       </c>
       <c r="M35">
-        <v>128.14400000000001</v>
+        <v>128.02000000000001</v>
       </c>
       <c r="N35">
-        <v>127.343</v>
+        <v>127.66</v>
       </c>
       <c r="O35">
-        <v>127.452</v>
+        <v>127.5</v>
       </c>
       <c r="P35">
-        <v>127.712</v>
+        <v>127.54</v>
       </c>
       <c r="Q35">
-        <v>128.06800000000001</v>
+        <v>128.04</v>
       </c>
       <c r="R35">
-        <v>127.95099999999999</v>
+        <v>128.41999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -7628,37 +7629,37 @@
         <v>162</v>
       </c>
       <c r="H36">
-        <v>104.721</v>
+        <v>104.59</v>
       </c>
       <c r="I36">
-        <v>104.72199999999999</v>
+        <v>104.66</v>
       </c>
       <c r="J36">
-        <v>104.57299999999999</v>
+        <v>104.59</v>
       </c>
       <c r="K36">
-        <v>104.744</v>
+        <v>104.67</v>
       </c>
       <c r="L36">
-        <v>104.254</v>
+        <v>104.43</v>
       </c>
       <c r="M36">
-        <v>104.036</v>
+        <v>103.97</v>
       </c>
       <c r="N36">
-        <v>103.352</v>
+        <v>103.64</v>
       </c>
       <c r="O36">
-        <v>103.407</v>
+        <v>103.51</v>
       </c>
       <c r="P36">
-        <v>103.69</v>
+        <v>103.51</v>
       </c>
       <c r="Q36">
-        <v>104.01600000000001</v>
+        <v>104.02</v>
       </c>
       <c r="R36">
-        <v>103.89700000000001</v>
+        <v>104.35</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -7684,37 +7685,37 @@
         <v>166</v>
       </c>
       <c r="H37">
-        <v>97.031999999999996</v>
+        <v>96.7</v>
       </c>
       <c r="I37">
-        <v>97.043000000000006</v>
+        <v>96.91</v>
       </c>
       <c r="J37">
-        <v>96.899000000000001</v>
+        <v>96.98</v>
       </c>
       <c r="K37">
-        <v>97.108000000000004</v>
+        <v>96.96</v>
       </c>
       <c r="L37">
-        <v>96.570999999999998</v>
+        <v>96.76</v>
       </c>
       <c r="M37">
-        <v>96.361000000000004</v>
+        <v>96.28</v>
       </c>
       <c r="N37">
-        <v>95.644999999999996</v>
+        <v>95.98</v>
       </c>
       <c r="O37">
-        <v>95.747</v>
+        <v>95.73</v>
       </c>
       <c r="P37">
-        <v>96.066999999999993</v>
+        <v>95.9</v>
       </c>
       <c r="Q37">
-        <v>96.409000000000006</v>
+        <v>96.46</v>
       </c>
       <c r="R37">
-        <v>96.265000000000001</v>
+        <v>96.75</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -7740,37 +7741,37 @@
         <v>170</v>
       </c>
       <c r="H38">
-        <v>90.349000000000004</v>
+        <v>90.22</v>
       </c>
       <c r="I38">
-        <v>90.367999999999995</v>
+        <v>90.3</v>
       </c>
       <c r="J38">
-        <v>90.212000000000003</v>
+        <v>90.24</v>
       </c>
       <c r="K38">
-        <v>90.438999999999993</v>
+        <v>90.34</v>
       </c>
       <c r="L38">
-        <v>89.894999999999996</v>
+        <v>90.09</v>
       </c>
       <c r="M38">
-        <v>89.677000000000007</v>
+        <v>89.59</v>
       </c>
       <c r="N38">
-        <v>88.97</v>
+        <v>89.28</v>
       </c>
       <c r="O38">
-        <v>89.07</v>
+        <v>89.17</v>
       </c>
       <c r="P38">
-        <v>89.402000000000001</v>
+        <v>89.18</v>
       </c>
       <c r="Q38">
-        <v>89.753</v>
+        <v>89.75</v>
       </c>
       <c r="R38">
-        <v>89.602000000000004</v>
+        <v>90.13</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -7796,37 +7797,37 @@
         <v>174</v>
       </c>
       <c r="H39">
-        <v>98.177000000000007</v>
+        <v>98.02</v>
       </c>
       <c r="I39">
-        <v>98.197999999999993</v>
+        <v>98.13</v>
       </c>
       <c r="J39">
-        <v>98.02</v>
+        <v>98.03</v>
       </c>
       <c r="K39">
-        <v>98.254999999999995</v>
+        <v>98.14</v>
       </c>
       <c r="L39">
-        <v>97.667000000000002</v>
+        <v>97.87</v>
       </c>
       <c r="M39">
-        <v>97.438999999999993</v>
+        <v>97.33</v>
       </c>
       <c r="N39">
-        <v>96.665000000000006</v>
+        <v>96.99</v>
       </c>
       <c r="O39">
-        <v>96.787000000000006</v>
+        <v>96.88</v>
       </c>
       <c r="P39">
-        <v>97.14</v>
+        <v>96.99</v>
       </c>
       <c r="Q39">
-        <v>97.522000000000006</v>
+        <v>97.51</v>
       </c>
       <c r="R39">
-        <v>97.349000000000004</v>
+        <v>97.91</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -7852,37 +7853,37 @@
         <v>178</v>
       </c>
       <c r="H40">
-        <v>97.596000000000004</v>
+        <v>97.43</v>
       </c>
       <c r="I40">
-        <v>97.613</v>
+        <v>97.53</v>
       </c>
       <c r="J40">
-        <v>97.423000000000002</v>
+        <v>97.43</v>
       </c>
       <c r="K40">
-        <v>97.676000000000002</v>
+        <v>97.54</v>
       </c>
       <c r="L40">
-        <v>97.072000000000003</v>
+        <v>97.28</v>
       </c>
       <c r="M40">
-        <v>96.831000000000003</v>
+        <v>96.71</v>
       </c>
       <c r="N40">
-        <v>96.037999999999997</v>
+        <v>96.37</v>
       </c>
       <c r="O40">
-        <v>96.173000000000002</v>
+        <v>96.27</v>
       </c>
       <c r="P40">
-        <v>96.555999999999997</v>
+        <v>96.39</v>
       </c>
       <c r="Q40">
-        <v>96.956000000000003</v>
+        <v>96.94</v>
       </c>
       <c r="R40">
-        <v>96.775000000000006</v>
+        <v>97.36</v>
       </c>
     </row>
   </sheetData>
@@ -7904,168 +7905,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>